<commit_message>
Krieger des lichts fix
</commit_message>
<xml_diff>
--- a/guide_ffxiv.xlsx
+++ b/guide_ffxiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\DevFFXIVPocketGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8208E349-E753-417E-A1D9-20661732F995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14481FF6-04B8-4578-AA8C-10E52942BC77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
+    <workbookView xWindow="76935" yWindow="5355" windowWidth="27825" windowHeight="13635" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -11520,10 +11520,10 @@
   <dimension ref="A1:BF388"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="Q158" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R329" sqref="R329"/>
+      <selection pane="bottomRight" activeCell="F147" sqref="F147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.453125" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
include enemy_id include 5.5. content include unknown sources for everything
</commit_message>
<xml_diff>
--- a/guide_ffxiv.xlsx
+++ b/guide_ffxiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\DevFFXIVPocketGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C36379-689D-46A7-9EC2-370B762B0505}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF736AB5-2FEA-403F-A779-7704050B45E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15435" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17498" uniqueCount="3501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17589" uniqueCount="3515">
   <si>
     <t>date:</t>
   </si>
@@ -10528,9 +10528,6 @@
     <t>Die Goldene Ebene von Paglth'an</t>
   </si>
   <si>
-    <t>die_goldeneebene_von_paglthan</t>
-  </si>
-  <si>
     <t>5.5</t>
   </si>
   <si>
@@ -10558,14 +10555,59 @@
     <t>Der Turm, Paradigmenbrecher</t>
   </si>
   <si>
-    <t>der_turm_paradigmenbrecher</t>
+    <t>ui/icon/112000/112433.tex</t>
+  </si>
+  <si>
+    <t>ui/icon/112000/112429.tex</t>
+  </si>
+  <si>
+    <t>ui/icon/112000/112430.tex</t>
+  </si>
+  <si>
+    <t>ui/icon/112000/112428.tex</t>
+  </si>
+  <si>
+    <t>ui/icon/112000/112431.tex</t>
+  </si>
+  <si>
+    <t>der_turm,_paradigmenbrecher</t>
+  </si>
+  <si>
+    <t>n4r3</t>
+  </si>
+  <si>
+    <t>die_goldene_ebene_von_paglthan</t>
+  </si>
+  <si>
+    <t>w4d1</t>
+  </si>
+  <si>
+    <t>n4fh</t>
+  </si>
+  <si>
+    <t>n4fh_2</t>
+  </si>
+  <si>
+    <t>Unreal</t>
+  </si>
+  <si>
+    <t>o1fa_3</t>
+  </si>
+  <si>
+    <t>['Diamant-Waffe']</t>
+  </si>
+  <si>
+    <t>['Herzbube', 'Hänsel &amp; Gretel', 'Hänsel', 'Gretel', 'Xun-Zi', 'Rotes Mädchen', 'Ihre Abgöttlichkeit', 'Ihre Infloreszenz']</t>
+  </si>
+  <si>
+    <t>['Amhuluk', 'Magitek-Reaktor', 'Luna-Bahamut']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10603,6 +10645,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -11556,10 +11604,10 @@
   <dimension ref="A1:BF393"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E313" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AW353" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F350" sqref="F350"/>
+      <selection pane="bottomRight" activeCell="AY368" sqref="AY368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -65087,22 +65135,32 @@
         <v>782</v>
       </c>
       <c r="F326" s="28" t="s">
+        <v>3506</v>
+      </c>
+      <c r="G326" s="28" t="s">
+        <v>3502</v>
+      </c>
+      <c r="H326" s="63" t="s">
         <v>3490</v>
       </c>
-      <c r="G326" s="28"/>
-      <c r="H326" s="63" t="s">
+      <c r="I326" s="28" t="s">
         <v>3491</v>
-      </c>
-      <c r="I326" s="28" t="s">
-        <v>3492</v>
       </c>
       <c r="J326" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="K326" s="67"/>
-      <c r="L326" s="77"/>
-      <c r="M326" s="32"/>
-      <c r="N326" s="32"/>
+      <c r="K326" s="67" t="s">
+        <v>1876</v>
+      </c>
+      <c r="L326" s="77">
+        <v>80</v>
+      </c>
+      <c r="M326" s="32">
+        <v>490</v>
+      </c>
+      <c r="N326" s="32">
+        <v>0</v>
+      </c>
       <c r="O326" s="30"/>
       <c r="P326" s="30"/>
       <c r="Q326" s="30"/>
@@ -65129,22 +65187,54 @@
       <c r="AL326" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="AM326" s="28"/>
-      <c r="AN326" s="28"/>
-      <c r="AO326" s="28"/>
-      <c r="AP326" s="28"/>
-      <c r="AQ326" s="28"/>
-      <c r="AR326" s="28"/>
-      <c r="AS326" s="28"/>
-      <c r="AT326" s="28"/>
-      <c r="AU326" s="28"/>
-      <c r="AV326" s="28"/>
-      <c r="AW326" s="28"/>
-      <c r="AX326" s="28"/>
-      <c r="AY326" s="28"/>
-      <c r="AZ326" s="28"/>
-      <c r="BA326" s="28"/>
-      <c r="BB326" s="28"/>
+      <c r="AM326" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AN326" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AO326" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AP326" s="28" t="s">
+        <v>889</v>
+      </c>
+      <c r="AQ326" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AR326" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AS326" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AT326" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AU326" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AV326" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AW326" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AX326" s="28" t="s">
+        <v>3507</v>
+      </c>
+      <c r="AY326" s="28" t="s">
+        <v>3514</v>
+      </c>
+      <c r="AZ326" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BA326" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BB326" s="28" t="s">
+        <v>941</v>
+      </c>
       <c r="BC326" s="28"/>
       <c r="BD326" s="28"/>
       <c r="BE326" s="28"/>
@@ -67303,7 +67393,7 @@
         <v>3354</v>
       </c>
       <c r="J340" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K340" s="67" t="s">
         <v>1876</v>
@@ -67475,7 +67565,7 @@
         <v>3354</v>
       </c>
       <c r="J341" s="28" t="s">
-        <v>76</v>
+        <v>2325</v>
       </c>
       <c r="K341" s="67" t="s">
         <v>1876</v>
@@ -67774,7 +67864,9 @@
       <c r="BE342" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="BF342" s="28"/>
+      <c r="BF342" s="28" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="343" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A343" s="28"/>
@@ -67785,28 +67877,38 @@
         <v>191</v>
       </c>
       <c r="D343" s="82" t="s">
-        <v>3493</v>
+        <v>3492</v>
       </c>
       <c r="E343" s="28" t="s">
         <v>782</v>
       </c>
       <c r="F343" s="82" t="s">
-        <v>3495</v>
-      </c>
-      <c r="G343" s="28"/>
+        <v>3494</v>
+      </c>
+      <c r="G343" s="28" t="s">
+        <v>3500</v>
+      </c>
       <c r="H343" s="63" t="s">
+        <v>3490</v>
+      </c>
+      <c r="I343" s="28" t="s">
         <v>3491</v>
       </c>
-      <c r="I343" s="28" t="s">
-        <v>3492</v>
-      </c>
       <c r="J343" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="K343" s="67"/>
-      <c r="L343" s="32"/>
-      <c r="M343" s="32"/>
-      <c r="N343" s="32"/>
+        <v>76</v>
+      </c>
+      <c r="K343" s="67" t="s">
+        <v>1876</v>
+      </c>
+      <c r="L343" s="32">
+        <v>80</v>
+      </c>
+      <c r="M343" s="32">
+        <v>495</v>
+      </c>
+      <c r="N343" s="32">
+        <v>0</v>
+      </c>
       <c r="O343" s="30"/>
       <c r="P343" s="30"/>
       <c r="Q343" s="30"/>
@@ -67833,22 +67935,54 @@
       <c r="AL343" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="AM343" s="28"/>
-      <c r="AN343" s="28"/>
-      <c r="AO343" s="28"/>
-      <c r="AP343" s="28"/>
-      <c r="AQ343" s="28"/>
-      <c r="AR343" s="28"/>
-      <c r="AS343" s="28"/>
-      <c r="AT343" s="28"/>
-      <c r="AU343" s="28"/>
-      <c r="AV343" s="28"/>
-      <c r="AW343" s="28"/>
-      <c r="AX343" s="28"/>
-      <c r="AY343" s="28"/>
-      <c r="AZ343" s="28"/>
-      <c r="BA343" s="28"/>
-      <c r="BB343" s="28"/>
+      <c r="AM343" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AN343" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AO343" s="28" t="s">
+        <v>889</v>
+      </c>
+      <c r="AP343" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AQ343" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AR343" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AS343" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AT343" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AU343" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AV343" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AW343" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AX343" s="28" t="s">
+        <v>3508</v>
+      </c>
+      <c r="AY343" s="28" t="s">
+        <v>3512</v>
+      </c>
+      <c r="AZ343" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BA343" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BB343" s="28" t="s">
+        <v>2293</v>
+      </c>
       <c r="BC343" s="28"/>
       <c r="BD343" s="28"/>
       <c r="BE343" s="28"/>
@@ -67863,28 +67997,38 @@
         <v>192</v>
       </c>
       <c r="D344" s="82" t="s">
-        <v>3494</v>
+        <v>3493</v>
       </c>
       <c r="E344" s="28" t="s">
         <v>782</v>
       </c>
       <c r="F344" s="82" t="s">
-        <v>3496</v>
-      </c>
-      <c r="G344" s="28"/>
+        <v>3495</v>
+      </c>
+      <c r="G344" s="28" t="s">
+        <v>3501</v>
+      </c>
       <c r="H344" s="63" t="s">
+        <v>3490</v>
+      </c>
+      <c r="I344" s="28" t="s">
         <v>3491</v>
       </c>
-      <c r="I344" s="28" t="s">
-        <v>3492</v>
-      </c>
       <c r="J344" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="K344" s="67"/>
-      <c r="L344" s="32"/>
-      <c r="M344" s="32"/>
-      <c r="N344" s="32"/>
+        <v>2325</v>
+      </c>
+      <c r="K344" s="67" t="s">
+        <v>1876</v>
+      </c>
+      <c r="L344" s="32">
+        <v>80</v>
+      </c>
+      <c r="M344" s="32">
+        <v>510</v>
+      </c>
+      <c r="N344" s="32">
+        <v>0</v>
+      </c>
       <c r="O344" s="30"/>
       <c r="P344" s="30"/>
       <c r="Q344" s="30"/>
@@ -67911,22 +68055,54 @@
       <c r="AL344" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="AM344" s="28"/>
-      <c r="AN344" s="28"/>
-      <c r="AO344" s="28"/>
-      <c r="AP344" s="28"/>
-      <c r="AQ344" s="28"/>
-      <c r="AR344" s="28"/>
-      <c r="AS344" s="28"/>
-      <c r="AT344" s="28"/>
-      <c r="AU344" s="28"/>
-      <c r="AV344" s="28"/>
-      <c r="AW344" s="28"/>
-      <c r="AX344" s="28"/>
-      <c r="AY344" s="28"/>
-      <c r="AZ344" s="28"/>
-      <c r="BA344" s="28"/>
-      <c r="BB344" s="28"/>
+      <c r="AM344" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AN344" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AO344" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AP344" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AQ344" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AR344" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AS344" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AT344" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AU344" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AV344" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AW344" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AX344" s="28" t="s">
+        <v>3509</v>
+      </c>
+      <c r="AY344" s="28" t="s">
+        <v>3512</v>
+      </c>
+      <c r="AZ344" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BA344" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BB344" s="28" t="s">
+        <v>2292</v>
+      </c>
       <c r="BC344" s="28"/>
       <c r="BD344" s="28"/>
       <c r="BE344" s="28"/>
@@ -67941,28 +68117,38 @@
         <v>193</v>
       </c>
       <c r="D345" s="82" t="s">
-        <v>3497</v>
+        <v>3496</v>
       </c>
       <c r="E345" s="28" t="s">
         <v>782</v>
       </c>
       <c r="F345" s="30" t="s">
-        <v>3498</v>
-      </c>
-      <c r="G345" s="28"/>
+        <v>3497</v>
+      </c>
+      <c r="G345" s="28" t="s">
+        <v>3499</v>
+      </c>
       <c r="H345" s="63" t="s">
+        <v>3490</v>
+      </c>
+      <c r="I345" s="28" t="s">
         <v>3491</v>
       </c>
-      <c r="I345" s="28" t="s">
-        <v>3492</v>
-      </c>
       <c r="J345" s="28" t="s">
-        <v>1922</v>
-      </c>
-      <c r="K345" s="67"/>
-      <c r="L345" s="32"/>
-      <c r="M345" s="32"/>
-      <c r="N345" s="32"/>
+        <v>3510</v>
+      </c>
+      <c r="K345" s="67" t="s">
+        <v>1876</v>
+      </c>
+      <c r="L345" s="32">
+        <v>80</v>
+      </c>
+      <c r="M345" s="32">
+        <v>430</v>
+      </c>
+      <c r="N345" s="32">
+        <v>435</v>
+      </c>
       <c r="O345" s="30"/>
       <c r="P345" s="30"/>
       <c r="Q345" s="30"/>
@@ -67989,22 +68175,54 @@
       <c r="AL345" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="AM345" s="28"/>
-      <c r="AN345" s="28"/>
-      <c r="AO345" s="28"/>
-      <c r="AP345" s="28"/>
-      <c r="AQ345" s="28"/>
-      <c r="AR345" s="28"/>
-      <c r="AS345" s="28"/>
-      <c r="AT345" s="28"/>
-      <c r="AU345" s="28"/>
-      <c r="AV345" s="28"/>
-      <c r="AW345" s="28"/>
-      <c r="AX345" s="28"/>
-      <c r="AY345" s="28"/>
-      <c r="AZ345" s="28"/>
-      <c r="BA345" s="28"/>
-      <c r="BB345" s="28"/>
+      <c r="AM345" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AN345" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AO345" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AP345" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AQ345" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AR345" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AS345" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AT345" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AU345" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AV345" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AW345" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AX345" s="28" t="s">
+        <v>3511</v>
+      </c>
+      <c r="AY345" s="28" t="s">
+        <v>1181</v>
+      </c>
+      <c r="AZ345" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BA345" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BB345" s="28" t="s">
+        <v>2333</v>
+      </c>
       <c r="BC345" s="28"/>
       <c r="BD345" s="28"/>
       <c r="BE345" s="28"/>
@@ -68423,28 +68641,38 @@
         <v>97</v>
       </c>
       <c r="D349" s="82" t="s">
-        <v>3499</v>
+        <v>3498</v>
       </c>
       <c r="E349" s="28" t="s">
         <v>782</v>
       </c>
       <c r="F349" s="28" t="s">
-        <v>3500</v>
-      </c>
-      <c r="G349" s="28"/>
-      <c r="H349" s="63" t="s">
+        <v>3504</v>
+      </c>
+      <c r="G349" s="28" t="s">
+        <v>3503</v>
+      </c>
+      <c r="H349" s="68" t="s">
+        <v>3490</v>
+      </c>
+      <c r="I349" s="28" t="s">
         <v>3491</v>
-      </c>
-      <c r="I349" s="28" t="s">
-        <v>3492</v>
       </c>
       <c r="J349" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="K349" s="32"/>
-      <c r="L349" s="32"/>
-      <c r="M349" s="32"/>
-      <c r="N349" s="32"/>
+      <c r="K349" s="32" t="s">
+        <v>1876</v>
+      </c>
+      <c r="L349" s="32">
+        <v>80</v>
+      </c>
+      <c r="M349" s="32">
+        <v>495</v>
+      </c>
+      <c r="N349" s="32">
+        <v>0</v>
+      </c>
       <c r="O349" s="30"/>
       <c r="P349" s="30"/>
       <c r="Q349" s="30"/>
@@ -68471,22 +68699,54 @@
       <c r="AL349" s="28" t="s">
         <v>574</v>
       </c>
-      <c r="AM349" s="28"/>
-      <c r="AN349" s="28"/>
-      <c r="AO349" s="28"/>
-      <c r="AP349" s="28"/>
-      <c r="AQ349" s="28"/>
-      <c r="AR349" s="28"/>
-      <c r="AS349" s="28"/>
-      <c r="AT349" s="28"/>
-      <c r="AU349" s="28"/>
-      <c r="AV349" s="28"/>
-      <c r="AW349" s="28"/>
-      <c r="AX349" s="28"/>
-      <c r="AY349" s="28"/>
-      <c r="AZ349" s="28"/>
-      <c r="BA349" s="28"/>
-      <c r="BB349" s="28"/>
+      <c r="AM349" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AN349" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AO349" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AP349" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AQ349" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AR349" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AS349" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AT349" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AU349" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AV349" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AW349" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AX349" s="28" t="s">
+        <v>3505</v>
+      </c>
+      <c r="AY349" s="28" t="s">
+        <v>3513</v>
+      </c>
+      <c r="AZ349" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BA349" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BB349" s="28" t="s">
+        <v>941</v>
+      </c>
       <c r="BC349" s="28"/>
       <c r="BD349" s="28"/>
       <c r="BE349" s="28"/>
@@ -75232,6 +75492,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:BF393" xr:uid="{A6EE1CE3-DC85-4AC8-ADB1-E8F1B02F8C62}"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="F281">
     <cfRule type="duplicateValues" dxfId="28" priority="33"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add quest and duty date to 5.5 content
</commit_message>
<xml_diff>
--- a/guide_ffxiv.xlsx
+++ b/guide_ffxiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\DevFFXIVPocketGuide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\DevFFXIVPocketGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF736AB5-2FEA-403F-A779-7704050B45E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FC0A51-3308-4551-BE5B-DE155750D790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15435" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15465" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,14 +36,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17589" uniqueCount="3515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17707" uniqueCount="3540">
   <si>
     <t>date:</t>
   </si>
@@ -10601,6 +10603,81 @@
   </si>
   <si>
     <t>['Amhuluk', 'Magitek-Reaktor', 'Luna-Bahamut']</t>
+  </si>
+  <si>
+    <t>The_Cloud_Deck</t>
+  </si>
+  <si>
+    <t>The_Cloud_Deck_(Extreme)</t>
+  </si>
+  <si>
+    <t>The_Whorleater_(Unreal)</t>
+  </si>
+  <si>
+    <t>The_Tower_at_Paradigm's_Breach</t>
+  </si>
+  <si>
+    <t>Paglth'an_(Duty)</t>
+  </si>
+  <si>
+    <t>Paglth'an</t>
+  </si>
+  <si>
+    <t>Luna-Bahamut</t>
+  </si>
+  <si>
+    <t>Seven Flames</t>
+  </si>
+  <si>
+    <t>A-Magitek-Prädator</t>
+  </si>
+  <si>
+    <t>Goldene Flammen</t>
+  </si>
+  <si>
+    <t>Des Schicksals grausam Ränke</t>
+  </si>
+  <si>
+    <t>Androiden</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>The Sound of the End</t>
+  </si>
+  <si>
+    <t>Emil (Despair)</t>
+  </si>
+  <si>
+    <t>Kainé (Final Fantasy Main Theme Version)</t>
+  </si>
+  <si>
+    <t>Mourning</t>
+  </si>
+  <si>
+    <t>The Sound of the End: 8bit</t>
+  </si>
+  <si>
+    <t>Maschinenwesen-Puppe</t>
+  </si>
+  <si>
+    <t>Aufzieh-9S</t>
+  </si>
+  <si>
+    <t>Diamant-Waffen</t>
+  </si>
+  <si>
+    <t>Diamant-Gwiber</t>
+  </si>
+  <si>
+    <t>In the Arms of War</t>
+  </si>
+  <si>
+    <t>Zeta-Diamant</t>
+  </si>
+  <si>
+    <t>Gleißendes Leben</t>
   </si>
 </sst>
 </file>
@@ -10994,7 +11071,37 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{1C4B43FA-7260-408A-8148-908495596B84}"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -11604,10 +11711,10 @@
   <dimension ref="A1:BF393"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AW353" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AX258" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY368" sqref="AY368"/>
+      <selection pane="bottomRight" activeCell="AY342" sqref="AY342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -63056,7 +63163,7 @@
       <c r="BE313" s="70"/>
       <c r="BF313" s="70"/>
     </row>
-    <row r="314" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A314" s="28"/>
       <c r="B314" s="29">
         <v>43644</v>
@@ -63228,7 +63335,7 @@
       </c>
       <c r="BF314" s="28"/>
     </row>
-    <row r="315" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A315" s="28"/>
       <c r="B315" s="29">
         <v>43644</v>
@@ -63400,7 +63507,7 @@
       </c>
       <c r="BF315" s="28"/>
     </row>
-    <row r="316" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A316" s="28"/>
       <c r="B316" s="29">
         <v>43644</v>
@@ -63572,7 +63679,7 @@
       </c>
       <c r="BF316" s="28"/>
     </row>
-    <row r="317" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A317" s="28"/>
       <c r="B317" s="29">
         <v>43644</v>
@@ -63744,7 +63851,7 @@
       </c>
       <c r="BF317" s="28"/>
     </row>
-    <row r="318" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A318" s="28"/>
       <c r="B318" s="29">
         <v>43644</v>
@@ -63916,7 +64023,7 @@
       </c>
       <c r="BF318" s="28"/>
     </row>
-    <row r="319" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A319" s="28"/>
       <c r="B319" s="29">
         <v>43644</v>
@@ -64088,7 +64195,7 @@
       </c>
       <c r="BF319" s="28"/>
     </row>
-    <row r="320" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A320" s="28"/>
       <c r="B320" s="29">
         <v>43644</v>
@@ -64260,7 +64367,7 @@
       </c>
       <c r="BF320" s="28"/>
     </row>
-    <row r="321" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A321" s="28"/>
       <c r="B321" s="29">
         <v>43644</v>
@@ -64432,7 +64539,7 @@
       </c>
       <c r="BF321" s="28"/>
     </row>
-    <row r="322" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A322" s="28"/>
       <c r="B322" s="29">
         <v>43767</v>
@@ -64604,7 +64711,7 @@
       </c>
       <c r="BF322" s="28"/>
     </row>
-    <row r="323" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A323" s="28"/>
       <c r="B323" s="29">
         <v>43848</v>
@@ -64776,7 +64883,7 @@
       </c>
       <c r="BF323" s="28"/>
     </row>
-    <row r="324" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A324" s="28"/>
       <c r="B324" s="29">
         <v>44054</v>
@@ -64948,7 +65055,7 @@
       </c>
       <c r="BF324" s="28"/>
     </row>
-    <row r="325" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A325" s="28"/>
       <c r="B325" s="29">
         <v>44173</v>
@@ -65120,7 +65227,7 @@
       </c>
       <c r="BF325" s="28"/>
     </row>
-    <row r="326" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A326" s="28"/>
       <c r="B326" s="29">
         <v>44299</v>
@@ -65161,29 +65268,69 @@
       <c r="N326" s="32">
         <v>0</v>
       </c>
-      <c r="O326" s="30"/>
+      <c r="O326" s="30" t="s">
+        <v>3524</v>
+      </c>
       <c r="P326" s="30"/>
       <c r="Q326" s="30"/>
-      <c r="R326" s="30"/>
-      <c r="S326" s="30"/>
-      <c r="T326" s="30"/>
-      <c r="U326" s="28"/>
-      <c r="V326" s="28"/>
-      <c r="W326" s="28"/>
-      <c r="X326" s="30"/>
-      <c r="Y326" s="30"/>
-      <c r="Z326" s="28"/>
-      <c r="AA326" s="28"/>
-      <c r="AB326" s="28"/>
+      <c r="R326" s="30" t="s">
+        <v>3520</v>
+      </c>
+      <c r="S326" s="30" t="s">
+        <v>3521</v>
+      </c>
+      <c r="T326" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="U326" s="28" t="s">
+        <v>3522</v>
+      </c>
+      <c r="V326" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="W326" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="X326" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="Y326" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="Z326" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AA326" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AB326" s="28" t="s">
+        <v>3179</v>
+      </c>
       <c r="AC326" s="33"/>
-      <c r="AD326" s="30"/>
-      <c r="AE326" s="30"/>
-      <c r="AF326" s="30"/>
-      <c r="AG326" s="28"/>
-      <c r="AH326" s="28"/>
-      <c r="AI326" s="28"/>
-      <c r="AJ326" s="28"/>
-      <c r="AK326" s="30"/>
+      <c r="AD326" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AE326" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AF326" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AG326" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AH326" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AI326" s="28" t="s">
+        <v>3523</v>
+      </c>
+      <c r="AJ326" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AK326" s="30" t="s">
+        <v>3179</v>
+      </c>
       <c r="AL326" s="28" t="s">
         <v>85</v>
       </c>
@@ -65235,12 +65382,18 @@
       <c r="BB326" s="28" t="s">
         <v>941</v>
       </c>
-      <c r="BC326" s="28"/>
-      <c r="BD326" s="28"/>
-      <c r="BE326" s="28"/>
+      <c r="BC326" s="28">
+        <v>77</v>
+      </c>
+      <c r="BD326" s="28">
+        <v>77</v>
+      </c>
+      <c r="BE326" s="28" t="s">
+        <v>3519</v>
+      </c>
       <c r="BF326" s="28"/>
     </row>
-    <row r="327" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A327" s="28" t="s">
         <v>779</v>
       </c>
@@ -67579,7 +67732,9 @@
       <c r="N341" s="32">
         <v>0</v>
       </c>
-      <c r="O341" s="30"/>
+      <c r="O341" s="30" t="s">
+        <v>2342</v>
+      </c>
       <c r="P341" s="30" t="s">
         <v>2345</v>
       </c>
@@ -67794,16 +67949,30 @@
       <c r="AC342" s="28" t="s">
         <v>2055</v>
       </c>
-      <c r="AD342" s="28"/>
+      <c r="AD342" s="28" t="s">
+        <v>3179</v>
+      </c>
       <c r="AE342" s="28" t="s">
         <v>2056</v>
       </c>
-      <c r="AF342" s="28"/>
-      <c r="AG342" s="30"/>
-      <c r="AH342" s="30"/>
-      <c r="AI342" s="30"/>
-      <c r="AJ342" s="30"/>
-      <c r="AK342" s="30"/>
+      <c r="AF342" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AG342" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AH342" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AI342" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AJ342" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AK342" s="30" t="s">
+        <v>3179</v>
+      </c>
       <c r="AL342" s="28" t="s">
         <v>186</v>
       </c>
@@ -67909,29 +68078,71 @@
       <c r="N343" s="32">
         <v>0</v>
       </c>
-      <c r="O343" s="30"/>
-      <c r="P343" s="30"/>
-      <c r="Q343" s="30"/>
-      <c r="R343" s="30"/>
-      <c r="S343" s="30"/>
-      <c r="T343" s="30"/>
-      <c r="U343" s="30"/>
-      <c r="V343" s="30"/>
-      <c r="W343" s="30"/>
-      <c r="X343" s="30"/>
-      <c r="Y343" s="30"/>
-      <c r="Z343" s="30"/>
-      <c r="AA343" s="30"/>
-      <c r="AB343" s="30"/>
+      <c r="O343" s="30" t="s">
+        <v>3539</v>
+      </c>
+      <c r="P343" s="30" t="s">
+        <v>2344</v>
+      </c>
+      <c r="Q343" s="30" t="s">
+        <v>3436</v>
+      </c>
+      <c r="R343" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="S343" s="30" t="s">
+        <v>3535</v>
+      </c>
+      <c r="T343" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="U343" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="V343" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="W343" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="X343" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="Y343" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="Z343" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AA343" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AB343" s="30" t="s">
+        <v>3179</v>
+      </c>
       <c r="AC343" s="28"/>
-      <c r="AD343" s="28"/>
+      <c r="AD343" s="28" t="s">
+        <v>3179</v>
+      </c>
       <c r="AE343" s="28"/>
-      <c r="AF343" s="28"/>
-      <c r="AG343" s="30"/>
-      <c r="AH343" s="30"/>
-      <c r="AI343" s="30"/>
-      <c r="AJ343" s="30"/>
-      <c r="AK343" s="30"/>
+      <c r="AF343" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AG343" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AH343" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AI343" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AJ343" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AK343" s="28" t="s">
+        <v>3179</v>
+      </c>
       <c r="AL343" s="28" t="s">
         <v>186</v>
       </c>
@@ -67983,9 +68194,15 @@
       <c r="BB343" s="28" t="s">
         <v>2293</v>
       </c>
-      <c r="BC343" s="28"/>
-      <c r="BD343" s="28"/>
-      <c r="BE343" s="28"/>
+      <c r="BC343" s="28">
+        <v>20075</v>
+      </c>
+      <c r="BD343" s="28">
+        <v>20075</v>
+      </c>
+      <c r="BE343" s="28" t="s">
+        <v>3515</v>
+      </c>
       <c r="BF343" s="28"/>
     </row>
     <row r="344" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -68029,29 +68246,71 @@
       <c r="N344" s="32">
         <v>0</v>
       </c>
-      <c r="O344" s="30"/>
-      <c r="P344" s="30"/>
-      <c r="Q344" s="30"/>
-      <c r="R344" s="30"/>
-      <c r="S344" s="30"/>
-      <c r="T344" s="30"/>
-      <c r="U344" s="30"/>
-      <c r="V344" s="30"/>
-      <c r="W344" s="30"/>
-      <c r="X344" s="30"/>
-      <c r="Y344" s="30"/>
-      <c r="Z344" s="30"/>
-      <c r="AA344" s="30"/>
-      <c r="AB344" s="30"/>
+      <c r="O344" s="30" t="s">
+        <v>2342</v>
+      </c>
+      <c r="P344" s="30" t="s">
+        <v>2345</v>
+      </c>
+      <c r="Q344" s="30" t="s">
+        <v>2349</v>
+      </c>
+      <c r="R344" s="30" t="s">
+        <v>3538</v>
+      </c>
+      <c r="S344" s="30" t="s">
+        <v>3535</v>
+      </c>
+      <c r="T344" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="U344" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="V344" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="W344" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="X344" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="Y344" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="Z344" s="30" t="s">
+        <v>3537</v>
+      </c>
+      <c r="AA344" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AB344" s="28" t="s">
+        <v>3179</v>
+      </c>
       <c r="AC344" s="28"/>
-      <c r="AD344" s="28"/>
+      <c r="AD344" s="28" t="s">
+        <v>3179</v>
+      </c>
       <c r="AE344" s="28"/>
-      <c r="AF344" s="28"/>
-      <c r="AG344" s="30"/>
-      <c r="AH344" s="30"/>
-      <c r="AI344" s="30"/>
-      <c r="AJ344" s="30"/>
-      <c r="AK344" s="30"/>
+      <c r="AF344" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AG344" s="30" t="s">
+        <v>3536</v>
+      </c>
+      <c r="AH344" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AI344" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AJ344" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AK344" s="28" t="s">
+        <v>3179</v>
+      </c>
       <c r="AL344" s="28" t="s">
         <v>186</v>
       </c>
@@ -68103,9 +68362,15 @@
       <c r="BB344" s="28" t="s">
         <v>2292</v>
       </c>
-      <c r="BC344" s="28"/>
-      <c r="BD344" s="28"/>
-      <c r="BE344" s="28"/>
+      <c r="BC344" s="28">
+        <v>20076</v>
+      </c>
+      <c r="BD344" s="28">
+        <v>20076</v>
+      </c>
+      <c r="BE344" s="28" t="s">
+        <v>3516</v>
+      </c>
       <c r="BF344" s="28"/>
     </row>
     <row r="345" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -68149,29 +68414,71 @@
       <c r="N345" s="32">
         <v>435</v>
       </c>
-      <c r="O345" s="30"/>
-      <c r="P345" s="30"/>
-      <c r="Q345" s="30"/>
-      <c r="R345" s="30"/>
-      <c r="S345" s="30"/>
-      <c r="T345" s="30"/>
-      <c r="U345" s="30"/>
-      <c r="V345" s="30"/>
-      <c r="W345" s="30"/>
-      <c r="X345" s="30"/>
-      <c r="Y345" s="30"/>
-      <c r="Z345" s="30"/>
-      <c r="AA345" s="30"/>
-      <c r="AB345" s="30"/>
+      <c r="O345" s="30" t="s">
+        <v>2339</v>
+      </c>
+      <c r="P345" s="30" t="s">
+        <v>2347</v>
+      </c>
+      <c r="Q345" s="30" t="s">
+        <v>2351</v>
+      </c>
+      <c r="R345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="S345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="T345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="U345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="V345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="W345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="X345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="Y345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="Z345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AA345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AB345" s="30" t="s">
+        <v>3179</v>
+      </c>
       <c r="AC345" s="28"/>
-      <c r="AD345" s="28"/>
+      <c r="AD345" s="30" t="s">
+        <v>3179</v>
+      </c>
       <c r="AE345" s="28"/>
-      <c r="AF345" s="28"/>
-      <c r="AG345" s="30"/>
-      <c r="AH345" s="30"/>
-      <c r="AI345" s="30"/>
-      <c r="AJ345" s="30"/>
-      <c r="AK345" s="30"/>
+      <c r="AF345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AG345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AH345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AI345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AJ345" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AK345" s="30" t="s">
+        <v>3179</v>
+      </c>
       <c r="AL345" s="28" t="s">
         <v>186</v>
       </c>
@@ -68223,9 +68530,15 @@
       <c r="BB345" s="28" t="s">
         <v>2333</v>
       </c>
-      <c r="BC345" s="28"/>
-      <c r="BD345" s="28"/>
-      <c r="BE345" s="28"/>
+      <c r="BC345" s="28">
+        <v>64003</v>
+      </c>
+      <c r="BD345" s="28">
+        <v>64003</v>
+      </c>
+      <c r="BE345" s="28" t="s">
+        <v>3517</v>
+      </c>
       <c r="BF345" s="28"/>
     </row>
     <row r="346" spans="1:58" x14ac:dyDescent="0.25">
@@ -68290,7 +68603,7 @@
       <c r="BE346" s="28"/>
       <c r="BF346" s="28"/>
     </row>
-    <row r="347" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A347" s="28"/>
       <c r="B347" s="35">
         <v>43767</v>
@@ -68462,7 +68775,7 @@
       </c>
       <c r="BF347" s="28"/>
     </row>
-    <row r="348" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A348" s="28"/>
       <c r="B348" s="35">
         <v>44054</v>
@@ -68533,7 +68846,9 @@
       <c r="X348" s="28" t="s">
         <v>3302</v>
       </c>
-      <c r="Y348" s="28"/>
+      <c r="Y348" s="28" t="s">
+        <v>3179</v>
+      </c>
       <c r="Z348" s="30" t="s">
         <v>3179</v>
       </c>
@@ -68632,7 +68947,7 @@
       </c>
       <c r="BF348" s="28"/>
     </row>
-    <row r="349" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A349" s="28"/>
       <c r="B349" s="29">
         <v>44299</v>
@@ -68673,29 +68988,71 @@
       <c r="N349" s="32">
         <v>0</v>
       </c>
-      <c r="O349" s="30"/>
-      <c r="P349" s="30"/>
-      <c r="Q349" s="30"/>
-      <c r="R349" s="30"/>
-      <c r="S349" s="30"/>
-      <c r="T349" s="30"/>
-      <c r="U349" s="28"/>
-      <c r="V349" s="28"/>
-      <c r="W349" s="28"/>
-      <c r="X349" s="28"/>
-      <c r="Y349" s="28"/>
-      <c r="Z349" s="30"/>
-      <c r="AA349" s="30"/>
-      <c r="AB349" s="30"/>
+      <c r="O349" s="30" t="s">
+        <v>3525</v>
+      </c>
+      <c r="P349" s="30" t="s">
+        <v>1807</v>
+      </c>
+      <c r="Q349" s="30" t="s">
+        <v>2363</v>
+      </c>
+      <c r="R349" s="30" t="s">
+        <v>3526</v>
+      </c>
+      <c r="S349" s="30" t="s">
+        <v>3527</v>
+      </c>
+      <c r="T349" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="U349" s="28" t="s">
+        <v>3528</v>
+      </c>
+      <c r="V349" s="28" t="s">
+        <v>3529</v>
+      </c>
+      <c r="W349" s="28" t="s">
+        <v>3530</v>
+      </c>
+      <c r="X349" s="28" t="s">
+        <v>3531</v>
+      </c>
+      <c r="Y349" s="28" t="s">
+        <v>3532</v>
+      </c>
+      <c r="Z349" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AA349" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AB349" s="30" t="s">
+        <v>3179</v>
+      </c>
       <c r="AC349" s="33"/>
-      <c r="AD349" s="30"/>
+      <c r="AD349" s="30" t="s">
+        <v>3179</v>
+      </c>
       <c r="AE349" s="30"/>
-      <c r="AF349" s="30"/>
-      <c r="AG349" s="30"/>
-      <c r="AH349" s="30"/>
-      <c r="AI349" s="28"/>
-      <c r="AJ349" s="28"/>
-      <c r="AK349" s="30"/>
+      <c r="AF349" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AG349" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AH349" s="30" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AI349" s="28" t="s">
+        <v>3533</v>
+      </c>
+      <c r="AJ349" s="28" t="s">
+        <v>3534</v>
+      </c>
+      <c r="AK349" s="30" t="s">
+        <v>3179</v>
+      </c>
       <c r="AL349" s="28" t="s">
         <v>574</v>
       </c>
@@ -68747,12 +69104,18 @@
       <c r="BB349" s="28" t="s">
         <v>941</v>
       </c>
-      <c r="BC349" s="28"/>
-      <c r="BD349" s="28"/>
-      <c r="BE349" s="28"/>
+      <c r="BC349" s="28">
+        <v>30105</v>
+      </c>
+      <c r="BD349" s="28">
+        <v>30105</v>
+      </c>
+      <c r="BE349" s="28" t="s">
+        <v>3518</v>
+      </c>
       <c r="BF349" s="28"/>
     </row>
-    <row r="350" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A350" s="28"/>
       <c r="B350" s="35">
         <v>43662</v>
@@ -68924,7 +69287,7 @@
       </c>
       <c r="BF350" s="28"/>
     </row>
-    <row r="351" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A351" s="28"/>
       <c r="B351" s="35">
         <v>43662</v>
@@ -69096,7 +69459,7 @@
       </c>
       <c r="BF351" s="28"/>
     </row>
-    <row r="352" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A352" s="28"/>
       <c r="B352" s="35">
         <v>43662</v>
@@ -69268,7 +69631,7 @@
       </c>
       <c r="BF352" s="28"/>
     </row>
-    <row r="353" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A353" s="28"/>
       <c r="B353" s="35">
         <v>43662</v>
@@ -69440,7 +69803,7 @@
       </c>
       <c r="BF353" s="28"/>
     </row>
-    <row r="354" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A354" s="28"/>
       <c r="B354" s="35">
         <v>43676</v>
@@ -69612,7 +69975,7 @@
       </c>
       <c r="BF354" s="28"/>
     </row>
-    <row r="355" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A355" s="28"/>
       <c r="B355" s="35">
         <v>43676</v>
@@ -69784,7 +70147,7 @@
       </c>
       <c r="BF355" s="28"/>
     </row>
-    <row r="356" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A356" s="28"/>
       <c r="B356" s="35">
         <v>43676</v>
@@ -69956,7 +70319,7 @@
       </c>
       <c r="BF356" s="28"/>
     </row>
-    <row r="357" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A357" s="28"/>
       <c r="B357" s="35">
         <v>43676</v>
@@ -70128,7 +70491,7 @@
       </c>
       <c r="BF357" s="28"/>
     </row>
-    <row r="358" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A358" s="28"/>
       <c r="B358" s="35">
         <v>43848</v>
@@ -70300,7 +70663,7 @@
       </c>
       <c r="BF358" s="28"/>
     </row>
-    <row r="359" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A359" s="28"/>
       <c r="B359" s="35">
         <v>43848</v>
@@ -70472,7 +70835,7 @@
       </c>
       <c r="BF359" s="28"/>
     </row>
-    <row r="360" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A360" s="28"/>
       <c r="B360" s="35">
         <v>43848</v>
@@ -70644,7 +71007,7 @@
       </c>
       <c r="BF360" s="28"/>
     </row>
-    <row r="361" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A361" s="28"/>
       <c r="B361" s="35">
         <v>43848</v>
@@ -70816,7 +71179,7 @@
       </c>
       <c r="BF361" s="28"/>
     </row>
-    <row r="362" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A362" s="28"/>
       <c r="B362" s="35">
         <v>43848</v>
@@ -70988,7 +71351,7 @@
       </c>
       <c r="BF362" s="28"/>
     </row>
-    <row r="363" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A363" s="28"/>
       <c r="B363" s="35">
         <v>43848</v>
@@ -71160,7 +71523,7 @@
       </c>
       <c r="BF363" s="28"/>
     </row>
-    <row r="364" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A364" s="28"/>
       <c r="B364" s="35">
         <v>43848</v>
@@ -71332,7 +71695,7 @@
       </c>
       <c r="BF364" s="28"/>
     </row>
-    <row r="365" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A365" s="28"/>
       <c r="B365" s="35">
         <v>43848</v>
@@ -71504,7 +71867,7 @@
       </c>
       <c r="BF365" s="28"/>
     </row>
-    <row r="366" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A366" s="28"/>
       <c r="B366" s="35">
         <v>44173</v>
@@ -71674,7 +72037,7 @@
       </c>
       <c r="BF366" s="28"/>
     </row>
-    <row r="367" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:58" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A367" s="28"/>
       <c r="B367" s="35">
         <v>44173</v>
@@ -71846,7 +72209,7 @@
       </c>
       <c r="BF367" s="28"/>
     </row>
-    <row r="368" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A368" s="28"/>
       <c r="B368" s="35">
         <v>44173</v>
@@ -72018,7 +72381,7 @@
       </c>
       <c r="BF368" s="28"/>
     </row>
-    <row r="369" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A369" s="28"/>
       <c r="B369" s="35">
         <v>44173</v>
@@ -72190,7 +72553,7 @@
       </c>
       <c r="BF369" s="28"/>
     </row>
-    <row r="370" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A370" s="28"/>
       <c r="B370" s="35">
         <v>44173</v>
@@ -72362,7 +72725,7 @@
       </c>
       <c r="BF370" s="28"/>
     </row>
-    <row r="371" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A371" s="28"/>
       <c r="B371" s="35">
         <v>44173</v>
@@ -72534,7 +72897,7 @@
       </c>
       <c r="BF371" s="28"/>
     </row>
-    <row r="372" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A372" s="28"/>
       <c r="B372" s="35">
         <v>44173</v>
@@ -72706,7 +73069,7 @@
       </c>
       <c r="BF372" s="28"/>
     </row>
-    <row r="373" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:58" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A373" s="28"/>
       <c r="B373" s="35">
         <v>44173</v>
@@ -72878,7 +73241,7 @@
       </c>
       <c r="BF373" s="28"/>
     </row>
-    <row r="374" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A374" s="28"/>
       <c r="B374" s="35">
         <v>43781</v>
@@ -73050,7 +73413,7 @@
       </c>
       <c r="BF374" s="28"/>
     </row>
-    <row r="375" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A375" s="28" t="s">
         <v>781</v>
       </c>
@@ -75494,91 +75857,100 @@
   <autoFilter ref="A1:BF393" xr:uid="{A6EE1CE3-DC85-4AC8-ADB1-E8F1B02F8C62}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="F281">
-    <cfRule type="duplicateValues" dxfId="28" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F346 F328">
-    <cfRule type="duplicateValues" dxfId="27" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F375">
-    <cfRule type="duplicateValues" dxfId="26" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F347">
+    <cfRule type="duplicateValues" dxfId="28" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F348:F355">
+    <cfRule type="duplicateValues" dxfId="27" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F100">
+    <cfRule type="duplicateValues" dxfId="26" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F86:F99">
     <cfRule type="duplicateValues" dxfId="25" priority="29"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F348:F355">
+  <conditionalFormatting sqref="F194">
     <cfRule type="duplicateValues" dxfId="24" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F100">
+  <conditionalFormatting sqref="F287">
     <cfRule type="duplicateValues" dxfId="23" priority="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F86:F99">
+  <conditionalFormatting sqref="F392 F300:F312 F385:F389">
     <cfRule type="duplicateValues" dxfId="22" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F194">
+  <conditionalFormatting sqref="F284:F286">
     <cfRule type="duplicateValues" dxfId="21" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F287">
+  <conditionalFormatting sqref="F193">
     <cfRule type="duplicateValues" dxfId="20" priority="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F392 F300:F312 F385:F389">
+  <conditionalFormatting sqref="F356:F374">
     <cfRule type="duplicateValues" dxfId="19" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F284:F286">
-    <cfRule type="duplicateValues" dxfId="18" priority="22"/>
+  <conditionalFormatting sqref="F322:F326">
+    <cfRule type="duplicateValues" dxfId="18" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F193">
-    <cfRule type="duplicateValues" dxfId="17" priority="21"/>
+  <conditionalFormatting sqref="F377">
+    <cfRule type="duplicateValues" dxfId="17" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F356:F374">
-    <cfRule type="duplicateValues" dxfId="16" priority="20"/>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="duplicateValues" dxfId="16" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F322:F326">
+  <conditionalFormatting sqref="F288:F299">
     <cfRule type="duplicateValues" dxfId="15" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F377">
+  <conditionalFormatting sqref="F390:F391">
     <cfRule type="duplicateValues" dxfId="14" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2">
-    <cfRule type="duplicateValues" dxfId="13" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F288:F299">
-    <cfRule type="duplicateValues" dxfId="12" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F390:F391">
-    <cfRule type="duplicateValues" dxfId="11" priority="14"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F313">
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F163:F182">
-    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O378:O379">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O369">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O342:O345">
+  <conditionalFormatting sqref="O342:O343">
+    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O384">
+    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O379:O382">
+    <cfRule type="duplicateValues" dxfId="7" priority="55"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O382">
     <cfRule type="duplicateValues" dxfId="6" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O384">
+  <conditionalFormatting sqref="O381">
     <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O379:O382">
-    <cfRule type="duplicateValues" dxfId="4" priority="52"/>
+  <conditionalFormatting sqref="F393:F1048576 F1 F327 F3:F85 F101:F162 F195:F280 F282:F283 F314:F321 F183:F192">
+    <cfRule type="duplicateValues" dxfId="4" priority="65"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O382">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  <conditionalFormatting sqref="O385:O1048576 O346:O368 O383 O370:O377 O1:O340">
+    <cfRule type="duplicateValues" dxfId="3" priority="75"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O381">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  <conditionalFormatting sqref="O345">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F393:F1048576 F1 F327 F3:F85 F101:F162 F195:F280 F282:F283 F314:F321 F183:F192">
-    <cfRule type="duplicateValues" dxfId="1" priority="62"/>
+  <conditionalFormatting sqref="O341">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O385:O1048576 O346:O368 O383 O370:O377 O1:O341">
-    <cfRule type="duplicateValues" dxfId="0" priority="72"/>
+  <conditionalFormatting sqref="O344">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix issues with unknown sources element
</commit_message>
<xml_diff>
--- a/guide_ffxiv.xlsx
+++ b/guide_ffxiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\DevFFXIVPocketGuide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\DevFFXIVPocketGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FC0A51-3308-4551-BE5B-DE155750D790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB27196-6FDA-43C1-B6B1-ECCA77284279}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15465" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15315" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,14 +34,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -58,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17707" uniqueCount="3540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17724" uniqueCount="3540">
   <si>
     <t>date:</t>
   </si>
@@ -11711,10 +11709,10 @@
   <dimension ref="A1:BF393"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AX258" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AZ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY342" sqref="AY342"/>
+      <selection pane="bottomRight" activeCell="BF84" sqref="BF84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -25879,7 +25877,9 @@
       <c r="BE84" s="6" t="s">
         <v>3132</v>
       </c>
-      <c r="BF84" s="6"/>
+      <c r="BF84" s="6" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="85" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
@@ -42336,7 +42336,9 @@
       <c r="BE184" s="14" t="s">
         <v>3133</v>
       </c>
-      <c r="BF184" s="14"/>
+      <c r="BF184" s="14" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="185" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A185" s="14"/>
@@ -42506,7 +42508,9 @@
         <v>40010</v>
       </c>
       <c r="BE185" s="14"/>
-      <c r="BF185" s="14"/>
+      <c r="BF185" s="14" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="186" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A186" s="14"/>
@@ -42676,7 +42680,9 @@
         <v>40008</v>
       </c>
       <c r="BE186" s="14"/>
-      <c r="BF186" s="14"/>
+      <c r="BF186" s="14" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="187" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A187" s="14"/>
@@ -42848,7 +42854,9 @@
       <c r="BE187" s="14" t="s">
         <v>3134</v>
       </c>
-      <c r="BF187" s="14"/>
+      <c r="BF187" s="14" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="188" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A188" s="14"/>
@@ -43018,7 +43026,9 @@
         <v>40014</v>
       </c>
       <c r="BE188" s="14"/>
-      <c r="BF188" s="14"/>
+      <c r="BF188" s="14" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="189" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" s="14"/>
@@ -43188,7 +43198,9 @@
         <v>40018</v>
       </c>
       <c r="BE189" s="14"/>
-      <c r="BF189" s="14"/>
+      <c r="BF189" s="14" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="190" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A190" s="14"/>
@@ -43358,7 +43370,9 @@
         <v>40016</v>
       </c>
       <c r="BE190" s="14"/>
-      <c r="BF190" s="14"/>
+      <c r="BF190" s="14" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="191" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" s="14"/>
@@ -43528,7 +43542,9 @@
         <v>40021</v>
       </c>
       <c r="BE191" s="14"/>
-      <c r="BF191" s="14"/>
+      <c r="BF191" s="14" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="192" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A192" s="14" t="s">
@@ -56421,7 +56437,9 @@
       <c r="BE270" s="20" t="s">
         <v>581</v>
       </c>
-      <c r="BF270" s="20"/>
+      <c r="BF270" s="20" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="271" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A271" s="20"/>
@@ -56591,7 +56609,9 @@
         <v>40025</v>
       </c>
       <c r="BE271" s="20"/>
-      <c r="BF271" s="20"/>
+      <c r="BF271" s="20" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="272" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A272" s="20"/>
@@ -56761,7 +56781,9 @@
         <v>40022</v>
       </c>
       <c r="BE272" s="20"/>
-      <c r="BF272" s="20"/>
+      <c r="BF272" s="20" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="273" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A273" s="20"/>
@@ -56931,7 +56953,9 @@
         <v>40023</v>
       </c>
       <c r="BE273" s="20"/>
-      <c r="BF273" s="20"/>
+      <c r="BF273" s="20" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="274" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A274" s="20"/>
@@ -57101,7 +57125,9 @@
         <v>40024</v>
       </c>
       <c r="BE274" s="20"/>
-      <c r="BF274" s="20"/>
+      <c r="BF274" s="20" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="275" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A275" s="20"/>
@@ -57271,7 +57297,9 @@
         <v>40026</v>
       </c>
       <c r="BE275" s="20"/>
-      <c r="BF275" s="20"/>
+      <c r="BF275" s="20" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="276" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A276" s="20"/>
@@ -57443,7 +57471,9 @@
       <c r="BE276" s="20" t="s">
         <v>3131</v>
       </c>
-      <c r="BF276" s="20"/>
+      <c r="BF276" s="20" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="277" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="20" t="s">
@@ -65455,7 +65485,7 @@
       <c r="BE327" s="28"/>
       <c r="BF327" s="28"/>
     </row>
-    <row r="328" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A328" s="28"/>
       <c r="B328" s="38">
         <v>43644</v>
@@ -65627,7 +65657,7 @@
       </c>
       <c r="BF328" s="28"/>
     </row>
-    <row r="329" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A329" s="28"/>
       <c r="B329" s="38">
         <v>43644</v>
@@ -65799,7 +65829,7 @@
       </c>
       <c r="BF329" s="28"/>
     </row>
-    <row r="330" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A330" s="28"/>
       <c r="B330" s="38">
         <v>43644</v>
@@ -65971,7 +66001,7 @@
       </c>
       <c r="BF330" s="28"/>
     </row>
-    <row r="331" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A331" s="28"/>
       <c r="B331" s="38">
         <v>43644</v>
@@ -66143,7 +66173,7 @@
       </c>
       <c r="BF331" s="28"/>
     </row>
-    <row r="332" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A332" s="28"/>
       <c r="B332" s="38">
         <v>43644</v>
@@ -66315,7 +66345,7 @@
       </c>
       <c r="BF332" s="28"/>
     </row>
-    <row r="333" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A333" s="28"/>
       <c r="B333" s="38">
         <v>43767</v>
@@ -66485,7 +66515,7 @@
       </c>
       <c r="BF333" s="28"/>
     </row>
-    <row r="334" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A334" s="28"/>
       <c r="B334" s="38">
         <v>43848</v>
@@ -66657,7 +66687,7 @@
       </c>
       <c r="BF334" s="28"/>
     </row>
-    <row r="335" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A335" s="28"/>
       <c r="B335" s="38">
         <v>43848</v>
@@ -66829,7 +66859,7 @@
       </c>
       <c r="BF335" s="28"/>
     </row>
-    <row r="336" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A336" s="28"/>
       <c r="B336" s="38">
         <v>43928</v>
@@ -67001,7 +67031,7 @@
       </c>
       <c r="BF336" s="28"/>
     </row>
-    <row r="337" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A337" s="28"/>
       <c r="B337" s="38">
         <v>44054</v>
@@ -67173,7 +67203,7 @@
       </c>
       <c r="BF337" s="28"/>
     </row>
-    <row r="338" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A338" s="28"/>
       <c r="B338" s="38">
         <v>44054</v>
@@ -67345,7 +67375,7 @@
       </c>
       <c r="BF338" s="28"/>
     </row>
-    <row r="339" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A339" s="28"/>
       <c r="B339" s="38">
         <v>44054</v>
@@ -67519,7 +67549,7 @@
         <v>2499</v>
       </c>
     </row>
-    <row r="340" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A340" s="28"/>
       <c r="B340" s="38">
         <v>44173</v>
@@ -67691,7 +67721,7 @@
       </c>
       <c r="BF340" s="28"/>
     </row>
-    <row r="341" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A341" s="28"/>
       <c r="B341" s="38">
         <v>44173</v>
@@ -67863,7 +67893,7 @@
       </c>
       <c r="BF341" s="28"/>
     </row>
-    <row r="342" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A342" s="28"/>
       <c r="B342" s="38">
         <v>44173</v>
@@ -68037,7 +68067,7 @@
         <v>2499</v>
       </c>
     </row>
-    <row r="343" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A343" s="28"/>
       <c r="B343" s="29">
         <v>44299</v>
@@ -68205,7 +68235,7 @@
       </c>
       <c r="BF343" s="28"/>
     </row>
-    <row r="344" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A344" s="28"/>
       <c r="B344" s="29">
         <v>44299</v>
@@ -68373,7 +68403,7 @@
       </c>
       <c r="BF344" s="28"/>
     </row>
-    <row r="345" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A345" s="28"/>
       <c r="B345" s="29">
         <v>44299</v>
@@ -68541,7 +68571,7 @@
       </c>
       <c r="BF345" s="28"/>
     </row>
-    <row r="346" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A346" s="28" t="s">
         <v>780</v>
       </c>
@@ -73643,7 +73673,9 @@
         <v>50006</v>
       </c>
       <c r="BE376" s="28"/>
-      <c r="BF376" s="28"/>
+      <c r="BF376" s="28" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="377" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A377" s="28" t="s">

</xml_diff>

<commit_message>
add guides für 5.5
</commit_message>
<xml_diff>
--- a/guide_ffxiv.xlsx
+++ b/guide_ffxiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\DevFFXIVPocketGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB27196-6FDA-43C1-B6B1-ECCA77284279}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D22280-DA5D-4807-B8B5-48B33859DB72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15315" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
+    <workbookView xWindow="1830" yWindow="2850" windowWidth="32640" windowHeight="15375" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17724" uniqueCount="3540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17729" uniqueCount="3546">
   <si>
     <t>date:</t>
   </si>
@@ -10676,6 +10676,24 @@
   </si>
   <si>
     <t>Gleißendes Leben</t>
+  </si>
+  <si>
+    <t>apFP4v_zcCg</t>
+  </si>
+  <si>
+    <t>XlMEzOaO_eQ</t>
+  </si>
+  <si>
+    <t>fM4Nz8-3I4A</t>
+  </si>
+  <si>
+    <t>kmNz10AGer0</t>
+  </si>
+  <si>
+    <t>Jmq-zDBcc0s</t>
+  </si>
+  <si>
+    <t>BED7fIMOzts</t>
   </si>
 </sst>
 </file>
@@ -11709,10 +11727,10 @@
   <dimension ref="A1:BF393"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AZ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="Y328" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BF84" sqref="BF84"/>
+      <selection pane="bottomRight" activeCell="AH339" sqref="AH339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -63193,7 +63211,7 @@
       <c r="BE313" s="70"/>
       <c r="BF313" s="70"/>
     </row>
-    <row r="314" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A314" s="28"/>
       <c r="B314" s="29">
         <v>43644</v>
@@ -63365,7 +63383,7 @@
       </c>
       <c r="BF314" s="28"/>
     </row>
-    <row r="315" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A315" s="28"/>
       <c r="B315" s="29">
         <v>43644</v>
@@ -63537,7 +63555,7 @@
       </c>
       <c r="BF315" s="28"/>
     </row>
-    <row r="316" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A316" s="28"/>
       <c r="B316" s="29">
         <v>43644</v>
@@ -63709,7 +63727,7 @@
       </c>
       <c r="BF316" s="28"/>
     </row>
-    <row r="317" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A317" s="28"/>
       <c r="B317" s="29">
         <v>43644</v>
@@ -63881,7 +63899,7 @@
       </c>
       <c r="BF317" s="28"/>
     </row>
-    <row r="318" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A318" s="28"/>
       <c r="B318" s="29">
         <v>43644</v>
@@ -64053,7 +64071,7 @@
       </c>
       <c r="BF318" s="28"/>
     </row>
-    <row r="319" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A319" s="28"/>
       <c r="B319" s="29">
         <v>43644</v>
@@ -64225,7 +64243,7 @@
       </c>
       <c r="BF319" s="28"/>
     </row>
-    <row r="320" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A320" s="28"/>
       <c r="B320" s="29">
         <v>43644</v>
@@ -64397,7 +64415,7 @@
       </c>
       <c r="BF320" s="28"/>
     </row>
-    <row r="321" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A321" s="28"/>
       <c r="B321" s="29">
         <v>43644</v>
@@ -64569,7 +64587,7 @@
       </c>
       <c r="BF321" s="28"/>
     </row>
-    <row r="322" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A322" s="28"/>
       <c r="B322" s="29">
         <v>43767</v>
@@ -64741,7 +64759,7 @@
       </c>
       <c r="BF322" s="28"/>
     </row>
-    <row r="323" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A323" s="28"/>
       <c r="B323" s="29">
         <v>43848</v>
@@ -64913,7 +64931,7 @@
       </c>
       <c r="BF323" s="28"/>
     </row>
-    <row r="324" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A324" s="28"/>
       <c r="B324" s="29">
         <v>44054</v>
@@ -65085,7 +65103,7 @@
       </c>
       <c r="BF324" s="28"/>
     </row>
-    <row r="325" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A325" s="28"/>
       <c r="B325" s="29">
         <v>44173</v>
@@ -65257,7 +65275,7 @@
       </c>
       <c r="BF325" s="28"/>
     </row>
-    <row r="326" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A326" s="28"/>
       <c r="B326" s="29">
         <v>44299</v>
@@ -65336,12 +65354,14 @@
       <c r="AB326" s="28" t="s">
         <v>3179</v>
       </c>
-      <c r="AC326" s="33"/>
+      <c r="AC326" s="33" t="s">
+        <v>3540</v>
+      </c>
       <c r="AD326" s="30" t="s">
         <v>3179</v>
       </c>
       <c r="AE326" s="30" t="s">
-        <v>3179</v>
+        <v>3544</v>
       </c>
       <c r="AF326" s="30" t="s">
         <v>3179</v>
@@ -65423,7 +65443,7 @@
       </c>
       <c r="BF326" s="28"/>
     </row>
-    <row r="327" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A327" s="28" t="s">
         <v>779</v>
       </c>
@@ -65485,7 +65505,7 @@
       <c r="BE327" s="28"/>
       <c r="BF327" s="28"/>
     </row>
-    <row r="328" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A328" s="28"/>
       <c r="B328" s="38">
         <v>43644</v>
@@ -65657,7 +65677,7 @@
       </c>
       <c r="BF328" s="28"/>
     </row>
-    <row r="329" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A329" s="28"/>
       <c r="B329" s="38">
         <v>43644</v>
@@ -65829,7 +65849,7 @@
       </c>
       <c r="BF329" s="28"/>
     </row>
-    <row r="330" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A330" s="28"/>
       <c r="B330" s="38">
         <v>43644</v>
@@ -66001,7 +66021,7 @@
       </c>
       <c r="BF330" s="28"/>
     </row>
-    <row r="331" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A331" s="28"/>
       <c r="B331" s="38">
         <v>43644</v>
@@ -66173,7 +66193,7 @@
       </c>
       <c r="BF331" s="28"/>
     </row>
-    <row r="332" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A332" s="28"/>
       <c r="B332" s="38">
         <v>43644</v>
@@ -66345,7 +66365,7 @@
       </c>
       <c r="BF332" s="28"/>
     </row>
-    <row r="333" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A333" s="28"/>
       <c r="B333" s="38">
         <v>43767</v>
@@ -66515,7 +66535,7 @@
       </c>
       <c r="BF333" s="28"/>
     </row>
-    <row r="334" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A334" s="28"/>
       <c r="B334" s="38">
         <v>43848</v>
@@ -66687,7 +66707,7 @@
       </c>
       <c r="BF334" s="28"/>
     </row>
-    <row r="335" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A335" s="28"/>
       <c r="B335" s="38">
         <v>43848</v>
@@ -66859,7 +66879,7 @@
       </c>
       <c r="BF335" s="28"/>
     </row>
-    <row r="336" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A336" s="28"/>
       <c r="B336" s="38">
         <v>43928</v>
@@ -67031,7 +67051,7 @@
       </c>
       <c r="BF336" s="28"/>
     </row>
-    <row r="337" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A337" s="28"/>
       <c r="B337" s="38">
         <v>44054</v>
@@ -67203,7 +67223,7 @@
       </c>
       <c r="BF337" s="28"/>
     </row>
-    <row r="338" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A338" s="28"/>
       <c r="B338" s="38">
         <v>44054</v>
@@ -67375,7 +67395,7 @@
       </c>
       <c r="BF338" s="28"/>
     </row>
-    <row r="339" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A339" s="28"/>
       <c r="B339" s="38">
         <v>44054</v>
@@ -67549,7 +67569,7 @@
         <v>2499</v>
       </c>
     </row>
-    <row r="340" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A340" s="28"/>
       <c r="B340" s="38">
         <v>44173</v>
@@ -67721,7 +67741,7 @@
       </c>
       <c r="BF340" s="28"/>
     </row>
-    <row r="341" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A341" s="28"/>
       <c r="B341" s="38">
         <v>44173</v>
@@ -67893,7 +67913,7 @@
       </c>
       <c r="BF341" s="28"/>
     </row>
-    <row r="342" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A342" s="28"/>
       <c r="B342" s="38">
         <v>44173</v>
@@ -68067,7 +68087,7 @@
         <v>2499</v>
       </c>
     </row>
-    <row r="343" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A343" s="28"/>
       <c r="B343" s="29">
         <v>44299</v>
@@ -68150,7 +68170,9 @@
       <c r="AB343" s="30" t="s">
         <v>3179</v>
       </c>
-      <c r="AC343" s="28"/>
+      <c r="AC343" s="28" t="s">
+        <v>3541</v>
+      </c>
       <c r="AD343" s="28" t="s">
         <v>3179</v>
       </c>
@@ -68235,7 +68257,7 @@
       </c>
       <c r="BF343" s="28"/>
     </row>
-    <row r="344" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A344" s="28"/>
       <c r="B344" s="29">
         <v>44299</v>
@@ -68322,7 +68344,9 @@
       <c r="AD344" s="28" t="s">
         <v>3179</v>
       </c>
-      <c r="AE344" s="28"/>
+      <c r="AE344" s="28" t="s">
+        <v>3543</v>
+      </c>
       <c r="AF344" s="28" t="s">
         <v>3179</v>
       </c>
@@ -68403,7 +68427,7 @@
       </c>
       <c r="BF344" s="28"/>
     </row>
-    <row r="345" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A345" s="28"/>
       <c r="B345" s="29">
         <v>44299</v>
@@ -68571,7 +68595,7 @@
       </c>
       <c r="BF345" s="28"/>
     </row>
-    <row r="346" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A346" s="28" t="s">
         <v>780</v>
       </c>
@@ -68633,7 +68657,7 @@
       <c r="BE346" s="28"/>
       <c r="BF346" s="28"/>
     </row>
-    <row r="347" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A347" s="28"/>
       <c r="B347" s="35">
         <v>43767</v>
@@ -68805,7 +68829,7 @@
       </c>
       <c r="BF347" s="28"/>
     </row>
-    <row r="348" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A348" s="28"/>
       <c r="B348" s="35">
         <v>44054</v>
@@ -68977,7 +69001,7 @@
       </c>
       <c r="BF348" s="28"/>
     </row>
-    <row r="349" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A349" s="28"/>
       <c r="B349" s="29">
         <v>44299</v>
@@ -69060,11 +69084,15 @@
       <c r="AB349" s="30" t="s">
         <v>3179</v>
       </c>
-      <c r="AC349" s="33"/>
+      <c r="AC349" s="33" t="s">
+        <v>3542</v>
+      </c>
       <c r="AD349" s="30" t="s">
         <v>3179</v>
       </c>
-      <c r="AE349" s="30"/>
+      <c r="AE349" s="30" t="s">
+        <v>3545</v>
+      </c>
       <c r="AF349" s="30" t="s">
         <v>3179</v>
       </c>
@@ -69145,7 +69173,7 @@
       </c>
       <c r="BF349" s="28"/>
     </row>
-    <row r="350" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A350" s="28"/>
       <c r="B350" s="35">
         <v>43662</v>
@@ -69317,7 +69345,7 @@
       </c>
       <c r="BF350" s="28"/>
     </row>
-    <row r="351" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A351" s="28"/>
       <c r="B351" s="35">
         <v>43662</v>
@@ -69489,7 +69517,7 @@
       </c>
       <c r="BF351" s="28"/>
     </row>
-    <row r="352" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A352" s="28"/>
       <c r="B352" s="35">
         <v>43662</v>
@@ -69661,7 +69689,7 @@
       </c>
       <c r="BF352" s="28"/>
     </row>
-    <row r="353" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A353" s="28"/>
       <c r="B353" s="35">
         <v>43662</v>
@@ -69833,7 +69861,7 @@
       </c>
       <c r="BF353" s="28"/>
     </row>
-    <row r="354" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A354" s="28"/>
       <c r="B354" s="35">
         <v>43676</v>
@@ -70005,7 +70033,7 @@
       </c>
       <c r="BF354" s="28"/>
     </row>
-    <row r="355" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A355" s="28"/>
       <c r="B355" s="35">
         <v>43676</v>
@@ -70177,7 +70205,7 @@
       </c>
       <c r="BF355" s="28"/>
     </row>
-    <row r="356" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A356" s="28"/>
       <c r="B356" s="35">
         <v>43676</v>
@@ -70349,7 +70377,7 @@
       </c>
       <c r="BF356" s="28"/>
     </row>
-    <row r="357" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A357" s="28"/>
       <c r="B357" s="35">
         <v>43676</v>
@@ -70521,7 +70549,7 @@
       </c>
       <c r="BF357" s="28"/>
     </row>
-    <row r="358" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A358" s="28"/>
       <c r="B358" s="35">
         <v>43848</v>
@@ -70693,7 +70721,7 @@
       </c>
       <c r="BF358" s="28"/>
     </row>
-    <row r="359" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A359" s="28"/>
       <c r="B359" s="35">
         <v>43848</v>
@@ -70865,7 +70893,7 @@
       </c>
       <c r="BF359" s="28"/>
     </row>
-    <row r="360" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A360" s="28"/>
       <c r="B360" s="35">
         <v>43848</v>
@@ -71037,7 +71065,7 @@
       </c>
       <c r="BF360" s="28"/>
     </row>
-    <row r="361" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A361" s="28"/>
       <c r="B361" s="35">
         <v>43848</v>
@@ -71209,7 +71237,7 @@
       </c>
       <c r="BF361" s="28"/>
     </row>
-    <row r="362" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A362" s="28"/>
       <c r="B362" s="35">
         <v>43848</v>
@@ -71381,7 +71409,7 @@
       </c>
       <c r="BF362" s="28"/>
     </row>
-    <row r="363" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A363" s="28"/>
       <c r="B363" s="35">
         <v>43848</v>
@@ -71553,7 +71581,7 @@
       </c>
       <c r="BF363" s="28"/>
     </row>
-    <row r="364" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A364" s="28"/>
       <c r="B364" s="35">
         <v>43848</v>
@@ -71725,7 +71753,7 @@
       </c>
       <c r="BF364" s="28"/>
     </row>
-    <row r="365" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A365" s="28"/>
       <c r="B365" s="35">
         <v>43848</v>
@@ -71897,7 +71925,7 @@
       </c>
       <c r="BF365" s="28"/>
     </row>
-    <row r="366" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A366" s="28"/>
       <c r="B366" s="35">
         <v>44173</v>
@@ -72067,7 +72095,7 @@
       </c>
       <c r="BF366" s="28"/>
     </row>
-    <row r="367" spans="1:58" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A367" s="28"/>
       <c r="B367" s="35">
         <v>44173</v>
@@ -72239,7 +72267,7 @@
       </c>
       <c r="BF367" s="28"/>
     </row>
-    <row r="368" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A368" s="28"/>
       <c r="B368" s="35">
         <v>44173</v>
@@ -72411,7 +72439,7 @@
       </c>
       <c r="BF368" s="28"/>
     </row>
-    <row r="369" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A369" s="28"/>
       <c r="B369" s="35">
         <v>44173</v>
@@ -72583,7 +72611,7 @@
       </c>
       <c r="BF369" s="28"/>
     </row>
-    <row r="370" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A370" s="28"/>
       <c r="B370" s="35">
         <v>44173</v>
@@ -72755,7 +72783,7 @@
       </c>
       <c r="BF370" s="28"/>
     </row>
-    <row r="371" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A371" s="28"/>
       <c r="B371" s="35">
         <v>44173</v>
@@ -72927,7 +72955,7 @@
       </c>
       <c r="BF371" s="28"/>
     </row>
-    <row r="372" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A372" s="28"/>
       <c r="B372" s="35">
         <v>44173</v>
@@ -73099,7 +73127,7 @@
       </c>
       <c r="BF372" s="28"/>
     </row>
-    <row r="373" spans="1:58" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A373" s="28"/>
       <c r="B373" s="35">
         <v>44173</v>
@@ -73271,7 +73299,7 @@
       </c>
       <c r="BF373" s="28"/>
     </row>
-    <row r="374" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A374" s="28"/>
       <c r="B374" s="35">
         <v>43781</v>
@@ -73443,7 +73471,7 @@
       </c>
       <c r="BF374" s="28"/>
     </row>
-    <row r="375" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A375" s="28" t="s">
         <v>781</v>
       </c>

</xml_diff>

<commit_message>
fix finding names + daily updates
</commit_message>
<xml_diff>
--- a/guide_ffxiv.xlsx
+++ b/guide_ffxiv.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\DevFFXIVPocketGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8308CA7-86B1-473C-BA3A-23C9157A631C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C38855-51B4-4176-A117-FF98846136C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40290" yWindow="4410" windowWidth="38310" windowHeight="15375" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
+    <workbookView xWindow="50145" yWindow="1470" windowWidth="33120" windowHeight="18420" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$BF$393</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$BF$395</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17729" uniqueCount="3546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17786" uniqueCount="3554">
   <si>
     <t>date:</t>
   </si>
@@ -10694,6 +10694,30 @@
   </si>
   <si>
     <t>['Nihil-Thanatos', 'Nihil-Ferdiad', 'Scathach', 'Diabolos']</t>
+  </si>
+  <si>
+    <t>Die Dalriada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zadnor-Hochebene </t>
+  </si>
+  <si>
+    <t xml:space="preserve">zadnor_hochebene </t>
+  </si>
+  <si>
+    <t>die_dalriada</t>
+  </si>
+  <si>
+    <t>'5.55</t>
+  </si>
+  <si>
+    <t>['Augur Der IV. Legion', 'Gebändigte Aaskrähe', 'Gebändigter Alkonost', 'Skorpion Der IV. Legion', 'Cuchulainn Der IV. Legion', 'Saunion', 'Dawon Junior', 'Diablo-Armament']</t>
+  </si>
+  <si>
+    <t>Zadnor</t>
+  </si>
+  <si>
+    <t>The_Dalriada</t>
   </si>
 </sst>
 </file>
@@ -11087,7 +11111,27 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{1C4B43FA-7260-408A-8148-908495596B84}"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -11724,13 +11768,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB88280F-F23E-48B4-9B91-E7EC59D48F52}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:BF393"/>
+  <dimension ref="A1:BF395"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AL83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AZ83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY137" sqref="AY137"/>
+      <selection pane="bottomRight" activeCell="BE384" sqref="BE384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -33976,7 +34020,7 @@
       <c r="BE134" s="14"/>
       <c r="BF134" s="14"/>
     </row>
-    <row r="135" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A135" s="14"/>
       <c r="B135" s="15">
         <v>42318</v>
@@ -34148,7 +34192,7 @@
       </c>
       <c r="BF135" s="14"/>
     </row>
-    <row r="136" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A136" s="14"/>
       <c r="B136" s="15">
         <v>42528</v>
@@ -34320,7 +34364,7 @@
       </c>
       <c r="BF136" s="14"/>
     </row>
-    <row r="137" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A137" s="14"/>
       <c r="B137" s="15">
         <v>42752</v>
@@ -34492,7 +34536,7 @@
       </c>
       <c r="BF137" s="14"/>
     </row>
-    <row r="138" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A138" s="14"/>
       <c r="B138" s="15">
         <v>42192</v>
@@ -34664,7 +34708,7 @@
       </c>
       <c r="BF138" s="14"/>
     </row>
-    <row r="139" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A139" s="14"/>
       <c r="B139" s="15">
         <v>42192</v>
@@ -34836,7 +34880,7 @@
       </c>
       <c r="BF139" s="14"/>
     </row>
-    <row r="140" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A140" s="14"/>
       <c r="B140" s="15">
         <v>42192</v>
@@ -35008,7 +35052,7 @@
       </c>
       <c r="BF140" s="14"/>
     </row>
-    <row r="141" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A141" s="14"/>
       <c r="B141" s="15">
         <v>42192</v>
@@ -35180,7 +35224,7 @@
       </c>
       <c r="BF141" s="14"/>
     </row>
-    <row r="142" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A142" s="14"/>
       <c r="B142" s="15">
         <v>42206</v>
@@ -35352,7 +35396,7 @@
       </c>
       <c r="BF142" s="14"/>
     </row>
-    <row r="143" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A143" s="14"/>
       <c r="B143" s="15">
         <v>42206</v>
@@ -35524,7 +35568,7 @@
       </c>
       <c r="BF143" s="14"/>
     </row>
-    <row r="144" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
       <c r="B144" s="15">
         <v>42206</v>
@@ -35696,7 +35740,7 @@
       </c>
       <c r="BF144" s="14"/>
     </row>
-    <row r="145" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A145" s="14"/>
       <c r="B145" s="15">
         <v>42206</v>
@@ -35868,7 +35912,7 @@
       </c>
       <c r="BF145" s="14"/>
     </row>
-    <row r="146" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A146" s="14"/>
       <c r="B146" s="15">
         <v>42423</v>
@@ -36040,7 +36084,7 @@
       </c>
       <c r="BF146" s="14"/>
     </row>
-    <row r="147" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A147" s="14"/>
       <c r="B147" s="15">
         <v>42423</v>
@@ -36212,7 +36256,7 @@
       </c>
       <c r="BF147" s="14"/>
     </row>
-    <row r="148" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A148" s="14"/>
       <c r="B148" s="15">
         <v>42423</v>
@@ -36384,7 +36428,7 @@
       </c>
       <c r="BF148" s="14"/>
     </row>
-    <row r="149" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A149" s="14"/>
       <c r="B149" s="15">
         <v>42423</v>
@@ -36556,7 +36600,7 @@
       </c>
       <c r="BF149" s="14"/>
     </row>
-    <row r="150" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A150" s="14"/>
       <c r="B150" s="15">
         <v>42423</v>
@@ -36728,7 +36772,7 @@
       </c>
       <c r="BF150" s="14"/>
     </row>
-    <row r="151" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A151" s="14"/>
       <c r="B151" s="15">
         <v>42423</v>
@@ -36900,7 +36944,7 @@
       </c>
       <c r="BF151" s="14"/>
     </row>
-    <row r="152" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A152" s="14"/>
       <c r="B152" s="15">
         <v>42423</v>
@@ -37072,7 +37116,7 @@
       </c>
       <c r="BF152" s="14"/>
     </row>
-    <row r="153" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A153" s="14"/>
       <c r="B153" s="15">
         <v>42423</v>
@@ -37244,7 +37288,7 @@
       </c>
       <c r="BF153" s="14"/>
     </row>
-    <row r="154" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A154" s="14"/>
       <c r="B154" s="15">
         <v>42640</v>
@@ -37416,7 +37460,7 @@
       </c>
       <c r="BF154" s="14"/>
     </row>
-    <row r="155" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A155" s="14"/>
       <c r="B155" s="15">
         <v>42640</v>
@@ -37588,7 +37632,7 @@
       </c>
       <c r="BF155" s="14"/>
     </row>
-    <row r="156" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A156" s="14"/>
       <c r="B156" s="15">
         <v>42640</v>
@@ -37760,7 +37804,7 @@
       </c>
       <c r="BF156" s="14"/>
     </row>
-    <row r="157" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A157" s="14"/>
       <c r="B157" s="15">
         <v>42640</v>
@@ -37932,7 +37976,7 @@
       </c>
       <c r="BF157" s="14"/>
     </row>
-    <row r="158" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A158" s="14"/>
       <c r="B158" s="15">
         <v>42640</v>
@@ -38104,7 +38148,7 @@
       </c>
       <c r="BF158" s="14"/>
     </row>
-    <row r="159" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A159" s="14"/>
       <c r="B159" s="15">
         <v>42640</v>
@@ -38276,7 +38320,7 @@
       </c>
       <c r="BF159" s="14"/>
     </row>
-    <row r="160" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A160" s="14"/>
       <c r="B160" s="15">
         <v>42640</v>
@@ -38448,7 +38492,7 @@
       </c>
       <c r="BF160" s="14"/>
     </row>
-    <row r="161" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A161" s="14"/>
       <c r="B161" s="15">
         <v>42640</v>
@@ -38620,7 +38664,7 @@
       </c>
       <c r="BF161" s="14"/>
     </row>
-    <row r="162" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
         <v>773</v>
       </c>
@@ -73767,7 +73811,7 @@
       <c r="BE377" s="28"/>
       <c r="BF377" s="28"/>
     </row>
-    <row r="378" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A378" s="28"/>
       <c r="B378" s="35">
         <v>44117</v>
@@ -73935,7 +73979,7 @@
       </c>
       <c r="BF378" s="28"/>
     </row>
-    <row r="379" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A379" s="28"/>
       <c r="B379" s="35">
         <v>44117</v>
@@ -74103,7 +74147,7 @@
       </c>
       <c r="BF379" s="28"/>
     </row>
-    <row r="380" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A380" s="28"/>
       <c r="B380" s="35">
         <v>44229</v>
@@ -74257,7 +74301,7 @@
       </c>
       <c r="BF380" s="28"/>
     </row>
-    <row r="381" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A381" s="28"/>
       <c r="B381" s="35">
         <v>44229</v>
@@ -74411,97 +74455,161 @@
       </c>
       <c r="BF381" s="28"/>
     </row>
-    <row r="382" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A382" s="35" t="s">
-        <v>3480</v>
-      </c>
-      <c r="B382" s="35"/>
-      <c r="C382" s="28"/>
-      <c r="D382" s="83"/>
-      <c r="E382" s="28"/>
-      <c r="F382" s="28"/>
+    <row r="382" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A382" s="28"/>
+      <c r="B382" s="35">
+        <v>44117</v>
+      </c>
+      <c r="C382" s="28">
+        <v>9</v>
+      </c>
+      <c r="D382" s="83" t="s">
+        <v>3547</v>
+      </c>
+      <c r="E382" s="28" t="s">
+        <v>782</v>
+      </c>
+      <c r="F382" s="28" t="s">
+        <v>3548</v>
+      </c>
       <c r="G382" s="28"/>
-      <c r="H382" s="59"/>
-      <c r="I382" s="28"/>
-      <c r="J382" s="28"/>
-      <c r="K382" s="28"/>
-      <c r="L382" s="28"/>
-      <c r="M382" s="28"/>
-      <c r="N382" s="28"/>
-      <c r="O382" s="32"/>
-      <c r="P382" s="32"/>
-      <c r="Q382" s="32"/>
+      <c r="H382" s="59" t="s">
+        <v>3550</v>
+      </c>
+      <c r="I382" s="28" t="s">
+        <v>3490</v>
+      </c>
+      <c r="J382" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="K382" s="28">
+        <v>71</v>
+      </c>
+      <c r="L382" s="28" t="s">
+        <v>1876</v>
+      </c>
+      <c r="M382" s="28">
+        <v>0</v>
+      </c>
+      <c r="N382" s="28">
+        <v>430</v>
+      </c>
+      <c r="O382" s="32" t="s">
+        <v>2747</v>
+      </c>
+      <c r="P382" s="32" t="s">
+        <v>2749</v>
+      </c>
+      <c r="Q382" s="32" t="s">
+        <v>2748</v>
+      </c>
       <c r="R382" s="32"/>
       <c r="S382" s="32"/>
       <c r="T382" s="32"/>
       <c r="U382" s="28"/>
-      <c r="V382" s="28"/>
-      <c r="W382" s="28"/>
-      <c r="X382" s="28"/>
-      <c r="Y382" s="28"/>
-      <c r="Z382" s="28"/>
-      <c r="AA382" s="28"/>
-      <c r="AB382" s="28"/>
-      <c r="AC382" s="28"/>
-      <c r="AD382" s="28"/>
+      <c r="V382" s="32"/>
+      <c r="W382" s="32"/>
+      <c r="X382" s="32"/>
+      <c r="Y382" s="32"/>
+      <c r="Z382" s="32"/>
+      <c r="AA382" s="32"/>
+      <c r="AB382" s="32"/>
+      <c r="AC382" s="32"/>
+      <c r="AD382" s="32"/>
       <c r="AE382" s="28"/>
-      <c r="AF382" s="28"/>
+      <c r="AF382" s="32"/>
       <c r="AG382" s="28"/>
-      <c r="AH382" s="28"/>
+      <c r="AH382" s="32"/>
       <c r="AI382" s="28"/>
-      <c r="AJ382" s="28"/>
-      <c r="AK382" s="28"/>
-      <c r="AL382" s="32"/>
-      <c r="AM382" s="28"/>
-      <c r="AN382" s="28"/>
-      <c r="AO382" s="28"/>
-      <c r="AP382" s="28"/>
-      <c r="AQ382" s="28"/>
-      <c r="AR382" s="28"/>
-      <c r="AS382" s="28"/>
-      <c r="AT382" s="28"/>
-      <c r="AU382" s="28"/>
-      <c r="AV382" s="28"/>
-      <c r="AW382" s="28"/>
-      <c r="AX382" s="28"/>
-      <c r="AY382" s="28"/>
-      <c r="AZ382" s="28"/>
-      <c r="BA382" s="28"/>
-      <c r="BB382" s="28"/>
+      <c r="AJ382" s="32"/>
+      <c r="AK382" s="32"/>
+      <c r="AL382" s="32" t="s">
+        <v>2751</v>
+      </c>
+      <c r="AM382" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AN382" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AO382" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AP382" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AQ382" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AR382" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AS382" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AT382" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AU382" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AV382" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AW382" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AX382" s="28" t="s">
+        <v>2744</v>
+      </c>
+      <c r="AY382" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="AZ382" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BA382" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BB382" s="28" t="s">
+        <v>941</v>
+      </c>
       <c r="BC382" s="28"/>
       <c r="BD382" s="28"/>
-      <c r="BE382" s="28"/>
+      <c r="BE382" s="28" t="s">
+        <v>3552</v>
+      </c>
       <c r="BF382" s="28"/>
     </row>
-    <row r="383" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A383" s="28"/>
       <c r="B383" s="35">
-        <v>43676</v>
+        <v>44117</v>
       </c>
       <c r="C383" s="28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D383" s="83" t="s">
-        <v>2754</v>
+        <v>3546</v>
       </c>
       <c r="E383" s="28" t="s">
         <v>782</v>
       </c>
-      <c r="F383" s="28" t="s">
-        <v>1397</v>
+      <c r="F383" s="83" t="s">
+        <v>3549</v>
       </c>
       <c r="G383" s="28"/>
       <c r="H383" s="59" t="s">
-        <v>2454</v>
+        <v>3550</v>
       </c>
       <c r="I383" s="28" t="s">
-        <v>820</v>
+        <v>3490</v>
       </c>
       <c r="J383" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K383" s="28">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="L383" s="28" t="s">
         <v>1876</v>
@@ -74510,45 +74618,41 @@
         <v>0</v>
       </c>
       <c r="N383" s="28">
-        <v>505</v>
-      </c>
-      <c r="O383" s="28" t="s">
-        <v>2370</v>
-      </c>
-      <c r="P383" s="28" t="s">
-        <v>2372</v>
-      </c>
-      <c r="Q383" s="28" t="s">
-        <v>2371</v>
-      </c>
-      <c r="R383" s="28" t="s">
-        <v>3178</v>
-      </c>
-      <c r="S383" s="28" t="s">
-        <v>3178</v>
-      </c>
-      <c r="T383" s="28" t="s">
-        <v>3178</v>
-      </c>
+        <v>430</v>
+      </c>
+      <c r="O383" s="32" t="s">
+        <v>2747</v>
+      </c>
+      <c r="P383" s="32" t="s">
+        <v>2749</v>
+      </c>
+      <c r="Q383" s="32" t="s">
+        <v>2748</v>
+      </c>
+      <c r="R383" s="32" t="s">
+        <v>3178</v>
+      </c>
+      <c r="S383" s="32"/>
+      <c r="T383" s="32"/>
       <c r="U383" s="28"/>
       <c r="V383" s="28"/>
       <c r="W383" s="28"/>
-      <c r="X383" s="28"/>
-      <c r="Y383" s="28"/>
-      <c r="Z383" s="28"/>
-      <c r="AA383" s="28"/>
-      <c r="AB383" s="28"/>
-      <c r="AC383" s="28"/>
-      <c r="AD383" s="28"/>
+      <c r="X383" s="32"/>
+      <c r="Y383" s="32"/>
+      <c r="Z383" s="32"/>
+      <c r="AA383" s="32"/>
+      <c r="AB383" s="32"/>
+      <c r="AC383" s="32"/>
+      <c r="AD383" s="32"/>
       <c r="AE383" s="28"/>
-      <c r="AF383" s="28"/>
-      <c r="AG383" s="28"/>
-      <c r="AH383" s="28"/>
+      <c r="AF383" s="32"/>
+      <c r="AG383" s="32"/>
+      <c r="AH383" s="32"/>
       <c r="AI383" s="28"/>
-      <c r="AJ383" s="28"/>
-      <c r="AK383" s="28"/>
-      <c r="AL383" s="28" t="s">
-        <v>1386</v>
+      <c r="AJ383" s="32"/>
+      <c r="AK383" s="32"/>
+      <c r="AL383" s="32" t="s">
+        <v>2751</v>
       </c>
       <c r="AM383" s="28" t="s">
         <v>888</v>
@@ -74584,10 +74688,10 @@
         <v>888</v>
       </c>
       <c r="AX383" s="28" t="s">
-        <v>1398</v>
+        <v>2744</v>
       </c>
       <c r="AY383" s="28" t="s">
-        <v>2870</v>
+        <v>3551</v>
       </c>
       <c r="AZ383" s="28" t="s">
         <v>941</v>
@@ -74598,68 +74702,36 @@
       <c r="BB383" s="28" t="s">
         <v>941</v>
       </c>
-      <c r="BC383" s="28">
-        <v>55006</v>
-      </c>
-      <c r="BD383" s="28">
-        <v>55006</v>
-      </c>
+      <c r="BC383" s="28"/>
+      <c r="BD383" s="28"/>
       <c r="BE383" s="28" t="s">
-        <v>3163</v>
+        <v>3553</v>
       </c>
       <c r="BF383" s="28"/>
     </row>
-    <row r="384" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A384" s="28"/>
-      <c r="B384" s="35">
-        <v>44173</v>
-      </c>
-      <c r="C384" s="28">
-        <v>0</v>
-      </c>
-      <c r="D384" s="83" t="s">
-        <v>3273</v>
-      </c>
-      <c r="E384" s="28" t="s">
-        <v>782</v>
-      </c>
-      <c r="F384" s="28" t="s">
-        <v>3385</v>
-      </c>
+    <row r="384" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A384" s="35" t="s">
+        <v>3480</v>
+      </c>
+      <c r="B384" s="35"/>
+      <c r="C384" s="28"/>
+      <c r="D384" s="83"/>
+      <c r="E384" s="28"/>
+      <c r="F384" s="28"/>
       <c r="G384" s="28"/>
-      <c r="H384" s="59" t="s">
-        <v>3354</v>
-      </c>
-      <c r="I384" s="28" t="s">
-        <v>3353</v>
-      </c>
-      <c r="J384" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="K384" s="28" t="s">
-        <v>3386</v>
-      </c>
-      <c r="L384" s="28">
-        <v>80</v>
-      </c>
-      <c r="M384" s="28">
-        <v>0</v>
-      </c>
-      <c r="N384" s="28">
-        <v>505</v>
-      </c>
-      <c r="O384" s="28" t="s">
-        <v>2370</v>
-      </c>
-      <c r="P384" s="28" t="s">
-        <v>2372</v>
-      </c>
-      <c r="Q384" s="28" t="s">
-        <v>2371</v>
-      </c>
-      <c r="R384" s="28"/>
-      <c r="S384" s="28"/>
-      <c r="T384" s="28"/>
+      <c r="H384" s="59"/>
+      <c r="I384" s="28"/>
+      <c r="J384" s="28"/>
+      <c r="K384" s="28"/>
+      <c r="L384" s="28"/>
+      <c r="M384" s="28"/>
+      <c r="N384" s="28"/>
+      <c r="O384" s="32"/>
+      <c r="P384" s="32"/>
+      <c r="Q384" s="32"/>
+      <c r="R384" s="32"/>
+      <c r="S384" s="32"/>
+      <c r="T384" s="32"/>
       <c r="U384" s="28"/>
       <c r="V384" s="28"/>
       <c r="W384" s="28"/>
@@ -74677,91 +74749,85 @@
       <c r="AI384" s="28"/>
       <c r="AJ384" s="28"/>
       <c r="AK384" s="28"/>
-      <c r="AL384" s="28" t="s">
-        <v>1386</v>
-      </c>
-      <c r="AM384" s="28" t="s">
-        <v>888</v>
-      </c>
-      <c r="AN384" s="28" t="s">
-        <v>888</v>
-      </c>
-      <c r="AO384" s="28" t="s">
-        <v>888</v>
-      </c>
-      <c r="AP384" s="28" t="s">
-        <v>888</v>
-      </c>
-      <c r="AQ384" s="28" t="s">
-        <v>888</v>
-      </c>
-      <c r="AR384" s="28" t="s">
-        <v>888</v>
-      </c>
-      <c r="AS384" s="28" t="s">
-        <v>888</v>
-      </c>
-      <c r="AT384" s="28" t="s">
-        <v>888</v>
-      </c>
-      <c r="AU384" s="28" t="s">
-        <v>888</v>
-      </c>
-      <c r="AV384" s="28" t="s">
-        <v>888</v>
-      </c>
-      <c r="AW384" s="28" t="s">
-        <v>888</v>
-      </c>
-      <c r="AX384" s="28" t="s">
-        <v>3387</v>
-      </c>
-      <c r="AY384" s="28" t="s">
-        <v>941</v>
-      </c>
-      <c r="AZ384" s="28" t="s">
-        <v>941</v>
-      </c>
-      <c r="BA384" s="28" t="s">
-        <v>941</v>
-      </c>
-      <c r="BB384" s="28" t="s">
-        <v>941</v>
-      </c>
-      <c r="BC384" s="28">
-        <v>55008</v>
-      </c>
-      <c r="BD384" s="28">
-        <v>55008</v>
-      </c>
-      <c r="BE384" s="28" t="s">
-        <v>941</v>
-      </c>
+      <c r="AL384" s="32"/>
+      <c r="AM384" s="28"/>
+      <c r="AN384" s="28"/>
+      <c r="AO384" s="28"/>
+      <c r="AP384" s="28"/>
+      <c r="AQ384" s="28"/>
+      <c r="AR384" s="28"/>
+      <c r="AS384" s="28"/>
+      <c r="AT384" s="28"/>
+      <c r="AU384" s="28"/>
+      <c r="AV384" s="28"/>
+      <c r="AW384" s="28"/>
+      <c r="AX384" s="28"/>
+      <c r="AY384" s="28"/>
+      <c r="AZ384" s="28"/>
+      <c r="BA384" s="28"/>
+      <c r="BB384" s="28"/>
+      <c r="BC384" s="28"/>
+      <c r="BD384" s="28"/>
+      <c r="BE384" s="28"/>
       <c r="BF384" s="28"/>
     </row>
-    <row r="385" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A385" s="28" t="s">
-        <v>1413</v>
-      </c>
-      <c r="B385" s="35"/>
-      <c r="C385" s="32"/>
-      <c r="D385" s="82"/>
-      <c r="E385" s="28"/>
-      <c r="F385" s="28"/>
+    <row r="385" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A385" s="28"/>
+      <c r="B385" s="35">
+        <v>43676</v>
+      </c>
+      <c r="C385" s="28">
+        <v>0</v>
+      </c>
+      <c r="D385" s="83" t="s">
+        <v>2754</v>
+      </c>
+      <c r="E385" s="28" t="s">
+        <v>782</v>
+      </c>
+      <c r="F385" s="28" t="s">
+        <v>1397</v>
+      </c>
       <c r="G385" s="28"/>
-      <c r="H385" s="31"/>
-      <c r="I385" s="28"/>
-      <c r="J385" s="28"/>
-      <c r="K385" s="32"/>
-      <c r="L385" s="32"/>
-      <c r="M385" s="32"/>
-      <c r="N385" s="32"/>
-      <c r="O385" s="32"/>
-      <c r="P385" s="32"/>
-      <c r="Q385" s="32"/>
-      <c r="R385" s="32"/>
-      <c r="S385" s="32"/>
-      <c r="T385" s="32"/>
+      <c r="H385" s="59" t="s">
+        <v>2454</v>
+      </c>
+      <c r="I385" s="28" t="s">
+        <v>820</v>
+      </c>
+      <c r="J385" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="K385" s="28">
+        <v>1</v>
+      </c>
+      <c r="L385" s="28" t="s">
+        <v>1876</v>
+      </c>
+      <c r="M385" s="28">
+        <v>0</v>
+      </c>
+      <c r="N385" s="28">
+        <v>505</v>
+      </c>
+      <c r="O385" s="28" t="s">
+        <v>2370</v>
+      </c>
+      <c r="P385" s="28" t="s">
+        <v>2372</v>
+      </c>
+      <c r="Q385" s="28" t="s">
+        <v>2371</v>
+      </c>
+      <c r="R385" s="28" t="s">
+        <v>3178</v>
+      </c>
+      <c r="S385" s="28" t="s">
+        <v>3178</v>
+      </c>
+      <c r="T385" s="28" t="s">
+        <v>3178</v>
+      </c>
       <c r="U385" s="28"/>
       <c r="V385" s="28"/>
       <c r="W385" s="28"/>
@@ -74770,8 +74836,8 @@
       <c r="Z385" s="28"/>
       <c r="AA385" s="28"/>
       <c r="AB385" s="28"/>
-      <c r="AC385" s="33"/>
-      <c r="AD385" s="33"/>
+      <c r="AC385" s="28"/>
+      <c r="AD385" s="28"/>
       <c r="AE385" s="28"/>
       <c r="AF385" s="28"/>
       <c r="AG385" s="28"/>
@@ -74779,371 +74845,259 @@
       <c r="AI385" s="28"/>
       <c r="AJ385" s="28"/>
       <c r="AK385" s="28"/>
-      <c r="AL385" s="28"/>
-      <c r="AM385" s="28"/>
-      <c r="AN385" s="28"/>
-      <c r="AO385" s="28"/>
-      <c r="AP385" s="28"/>
-      <c r="AQ385" s="28"/>
-      <c r="AR385" s="28"/>
-      <c r="AS385" s="28"/>
-      <c r="AT385" s="28"/>
-      <c r="AU385" s="28"/>
-      <c r="AV385" s="28"/>
-      <c r="AW385" s="28"/>
-      <c r="AX385" s="28"/>
-      <c r="AY385" s="28"/>
-      <c r="AZ385" s="28"/>
-      <c r="BA385" s="28"/>
-      <c r="BB385" s="28"/>
-      <c r="BC385" s="28"/>
-      <c r="BD385" s="28"/>
-      <c r="BE385" s="28"/>
+      <c r="AL385" s="28" t="s">
+        <v>1386</v>
+      </c>
+      <c r="AM385" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AN385" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AO385" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AP385" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AQ385" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AR385" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AS385" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AT385" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AU385" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AV385" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AW385" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AX385" s="28" t="s">
+        <v>1398</v>
+      </c>
+      <c r="AY385" s="28" t="s">
+        <v>2870</v>
+      </c>
+      <c r="AZ385" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BA385" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BB385" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BC385" s="28">
+        <v>55006</v>
+      </c>
+      <c r="BD385" s="28">
+        <v>55006</v>
+      </c>
+      <c r="BE385" s="28" t="s">
+        <v>3163</v>
+      </c>
       <c r="BF385" s="28"/>
     </row>
     <row r="386" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A386" s="70"/>
-      <c r="B386" s="71">
-        <v>43809</v>
-      </c>
-      <c r="C386" s="70">
-        <v>26</v>
-      </c>
-      <c r="D386" s="84" t="s">
-        <v>1835</v>
-      </c>
-      <c r="E386" s="70" t="s">
+      <c r="A386" s="28"/>
+      <c r="B386" s="35">
+        <v>44173</v>
+      </c>
+      <c r="C386" s="28">
+        <v>0</v>
+      </c>
+      <c r="D386" s="83" t="s">
+        <v>3273</v>
+      </c>
+      <c r="E386" s="28" t="s">
         <v>782</v>
       </c>
-      <c r="F386" s="70" t="s">
-        <v>1861</v>
-      </c>
-      <c r="G386" s="70" t="s">
-        <v>1865</v>
-      </c>
-      <c r="H386" s="75" t="s">
-        <v>2463</v>
-      </c>
-      <c r="I386" s="70" t="s">
-        <v>1417</v>
-      </c>
-      <c r="J386" s="70" t="s">
+      <c r="F386" s="28" t="s">
+        <v>3385</v>
+      </c>
+      <c r="G386" s="28"/>
+      <c r="H386" s="59" t="s">
+        <v>3354</v>
+      </c>
+      <c r="I386" s="28" t="s">
+        <v>3353</v>
+      </c>
+      <c r="J386" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="K386" s="72">
-        <v>60</v>
-      </c>
-      <c r="L386" s="72" t="s">
-        <v>2318</v>
-      </c>
-      <c r="M386" s="72">
+      <c r="K386" s="28" t="s">
+        <v>3386</v>
+      </c>
+      <c r="L386" s="28">
+        <v>80</v>
+      </c>
+      <c r="M386" s="28">
         <v>0</v>
       </c>
-      <c r="N386" s="72">
-        <v>0</v>
-      </c>
-      <c r="O386" s="76" t="s">
-        <v>1867</v>
-      </c>
-      <c r="P386" s="76" t="s">
-        <v>1868</v>
-      </c>
-      <c r="Q386" s="76" t="s">
-        <v>1869</v>
-      </c>
-      <c r="R386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="S386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="T386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="U386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="V386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="W386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="X386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="Y386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="Z386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AA386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AB386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AC386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AD386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AE386" s="70" t="s">
-        <v>2263</v>
-      </c>
-      <c r="AF386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AG386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AH386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AI386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AJ386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AK386" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AL386" s="70" t="s">
-        <v>1870</v>
-      </c>
-      <c r="AM386" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AN386" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AO386" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AP386" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AQ386" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AR386" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AS386" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AT386" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AU386" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AV386" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AW386" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AX386" s="70" t="s">
-        <v>2317</v>
-      </c>
-      <c r="AY386" s="70" t="s">
-        <v>2846</v>
-      </c>
-      <c r="AZ386" s="70" t="s">
-        <v>941</v>
-      </c>
-      <c r="BA386" s="70" t="s">
-        <v>941</v>
-      </c>
-      <c r="BB386" s="70" t="s">
-        <v>941</v>
-      </c>
-      <c r="BC386" s="70">
-        <v>35026</v>
-      </c>
-      <c r="BD386" s="70">
-        <v>35026</v>
-      </c>
-      <c r="BE386" s="70" t="s">
-        <v>1835</v>
-      </c>
-      <c r="BF386" s="70"/>
+      <c r="N386" s="28">
+        <v>505</v>
+      </c>
+      <c r="O386" s="28" t="s">
+        <v>2370</v>
+      </c>
+      <c r="P386" s="28" t="s">
+        <v>2372</v>
+      </c>
+      <c r="Q386" s="28" t="s">
+        <v>2371</v>
+      </c>
+      <c r="R386" s="28"/>
+      <c r="S386" s="28"/>
+      <c r="T386" s="28"/>
+      <c r="U386" s="28"/>
+      <c r="V386" s="28"/>
+      <c r="W386" s="28"/>
+      <c r="X386" s="28"/>
+      <c r="Y386" s="28"/>
+      <c r="Z386" s="28"/>
+      <c r="AA386" s="28"/>
+      <c r="AB386" s="28"/>
+      <c r="AC386" s="28"/>
+      <c r="AD386" s="28"/>
+      <c r="AE386" s="28"/>
+      <c r="AF386" s="28"/>
+      <c r="AG386" s="28"/>
+      <c r="AH386" s="28"/>
+      <c r="AI386" s="28"/>
+      <c r="AJ386" s="28"/>
+      <c r="AK386" s="28"/>
+      <c r="AL386" s="28" t="s">
+        <v>1386</v>
+      </c>
+      <c r="AM386" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AN386" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AO386" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AP386" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AQ386" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AR386" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AS386" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AT386" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AU386" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AV386" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AW386" s="28" t="s">
+        <v>888</v>
+      </c>
+      <c r="AX386" s="28" t="s">
+        <v>3387</v>
+      </c>
+      <c r="AY386" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="AZ386" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BA386" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BB386" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BC386" s="28">
+        <v>55008</v>
+      </c>
+      <c r="BD386" s="28">
+        <v>55008</v>
+      </c>
+      <c r="BE386" s="28" t="s">
+        <v>941</v>
+      </c>
+      <c r="BF386" s="28"/>
     </row>
-    <row r="387" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A387" s="70"/>
-      <c r="B387" s="71">
-        <v>43809</v>
-      </c>
-      <c r="C387" s="70">
-        <v>27</v>
-      </c>
-      <c r="D387" s="84" t="s">
-        <v>1836</v>
-      </c>
-      <c r="E387" s="70" t="s">
-        <v>782</v>
-      </c>
-      <c r="F387" s="70" t="s">
-        <v>1862</v>
-      </c>
-      <c r="G387" s="70" t="s">
-        <v>1865</v>
-      </c>
-      <c r="H387" s="75" t="s">
-        <v>2463</v>
-      </c>
-      <c r="I387" s="70" t="s">
-        <v>1417</v>
-      </c>
-      <c r="J387" s="70" t="s">
-        <v>75</v>
-      </c>
-      <c r="K387" s="72">
-        <v>60</v>
-      </c>
-      <c r="L387" s="72" t="s">
-        <v>2318</v>
-      </c>
-      <c r="M387" s="72">
-        <v>0</v>
-      </c>
-      <c r="N387" s="72">
-        <v>0</v>
-      </c>
-      <c r="O387" s="76" t="s">
-        <v>1867</v>
-      </c>
-      <c r="P387" s="76" t="s">
-        <v>1868</v>
-      </c>
-      <c r="Q387" s="76" t="s">
-        <v>1869</v>
-      </c>
-      <c r="R387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="S387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="T387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="U387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="V387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="W387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="X387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="Y387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="Z387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AA387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AB387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AC387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AD387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AE387" s="70" t="s">
-        <v>2263</v>
-      </c>
-      <c r="AF387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AG387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AH387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AI387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AJ387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AK387" s="76" t="s">
-        <v>3178</v>
-      </c>
-      <c r="AL387" s="70" t="s">
-        <v>1870</v>
-      </c>
-      <c r="AM387" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AN387" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AO387" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AP387" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AQ387" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AR387" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AS387" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AT387" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AU387" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AV387" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AW387" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="AX387" s="70" t="s">
-        <v>2317</v>
-      </c>
-      <c r="AY387" s="70" t="s">
-        <v>2847</v>
-      </c>
-      <c r="AZ387" s="70" t="s">
-        <v>941</v>
-      </c>
-      <c r="BA387" s="70" t="s">
-        <v>941</v>
-      </c>
-      <c r="BB387" s="70" t="s">
-        <v>941</v>
-      </c>
-      <c r="BC387" s="70">
-        <v>35027</v>
-      </c>
-      <c r="BD387" s="70">
-        <v>35027</v>
-      </c>
-      <c r="BE387" s="70" t="s">
-        <v>3159</v>
-      </c>
-      <c r="BF387" s="70"/>
+    <row r="387" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A387" s="28" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B387" s="35"/>
+      <c r="C387" s="32"/>
+      <c r="D387" s="82"/>
+      <c r="E387" s="28"/>
+      <c r="F387" s="28"/>
+      <c r="G387" s="28"/>
+      <c r="H387" s="31"/>
+      <c r="I387" s="28"/>
+      <c r="J387" s="28"/>
+      <c r="K387" s="32"/>
+      <c r="L387" s="32"/>
+      <c r="M387" s="32"/>
+      <c r="N387" s="32"/>
+      <c r="O387" s="32"/>
+      <c r="P387" s="32"/>
+      <c r="Q387" s="32"/>
+      <c r="R387" s="32"/>
+      <c r="S387" s="32"/>
+      <c r="T387" s="32"/>
+      <c r="U387" s="28"/>
+      <c r="V387" s="28"/>
+      <c r="W387" s="28"/>
+      <c r="X387" s="28"/>
+      <c r="Y387" s="28"/>
+      <c r="Z387" s="28"/>
+      <c r="AA387" s="28"/>
+      <c r="AB387" s="28"/>
+      <c r="AC387" s="33"/>
+      <c r="AD387" s="33"/>
+      <c r="AE387" s="28"/>
+      <c r="AF387" s="28"/>
+      <c r="AG387" s="28"/>
+      <c r="AH387" s="28"/>
+      <c r="AI387" s="28"/>
+      <c r="AJ387" s="28"/>
+      <c r="AK387" s="28"/>
+      <c r="AL387" s="28"/>
+      <c r="AM387" s="28"/>
+      <c r="AN387" s="28"/>
+      <c r="AO387" s="28"/>
+      <c r="AP387" s="28"/>
+      <c r="AQ387" s="28"/>
+      <c r="AR387" s="28"/>
+      <c r="AS387" s="28"/>
+      <c r="AT387" s="28"/>
+      <c r="AU387" s="28"/>
+      <c r="AV387" s="28"/>
+      <c r="AW387" s="28"/>
+      <c r="AX387" s="28"/>
+      <c r="AY387" s="28"/>
+      <c r="AZ387" s="28"/>
+      <c r="BA387" s="28"/>
+      <c r="BB387" s="28"/>
+      <c r="BC387" s="28"/>
+      <c r="BD387" s="28"/>
+      <c r="BE387" s="28"/>
+      <c r="BF387" s="28"/>
     </row>
     <row r="388" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A388" s="70"/>
@@ -75151,16 +75105,16 @@
         <v>43809</v>
       </c>
       <c r="C388" s="70">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D388" s="84" t="s">
-        <v>1837</v>
+        <v>1835</v>
       </c>
       <c r="E388" s="70" t="s">
         <v>782</v>
       </c>
       <c r="F388" s="70" t="s">
-        <v>1863</v>
+        <v>1861</v>
       </c>
       <c r="G388" s="70" t="s">
         <v>1865</v>
@@ -75295,7 +75249,7 @@
         <v>2317</v>
       </c>
       <c r="AY388" s="70" t="s">
-        <v>2848</v>
+        <v>2846</v>
       </c>
       <c r="AZ388" s="70" t="s">
         <v>941</v>
@@ -75307,13 +75261,13 @@
         <v>941</v>
       </c>
       <c r="BC388" s="70">
-        <v>35028</v>
+        <v>35026</v>
       </c>
       <c r="BD388" s="70">
-        <v>35028</v>
+        <v>35026</v>
       </c>
       <c r="BE388" s="70" t="s">
-        <v>3160</v>
+        <v>1835</v>
       </c>
       <c r="BF388" s="70"/>
     </row>
@@ -75323,16 +75277,16 @@
         <v>43809</v>
       </c>
       <c r="C389" s="70">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D389" s="84" t="s">
-        <v>1838</v>
+        <v>1836</v>
       </c>
       <c r="E389" s="70" t="s">
         <v>782</v>
       </c>
       <c r="F389" s="70" t="s">
-        <v>1864</v>
+        <v>1862</v>
       </c>
       <c r="G389" s="70" t="s">
         <v>1865</v>
@@ -75467,7 +75421,7 @@
         <v>2317</v>
       </c>
       <c r="AY389" s="70" t="s">
-        <v>2849</v>
+        <v>2847</v>
       </c>
       <c r="AZ389" s="70" t="s">
         <v>941</v>
@@ -75479,13 +75433,13 @@
         <v>941</v>
       </c>
       <c r="BC389" s="70">
-        <v>35029</v>
+        <v>35027</v>
       </c>
       <c r="BD389" s="70">
-        <v>35029</v>
+        <v>35027</v>
       </c>
       <c r="BE389" s="70" t="s">
-        <v>3161</v>
+        <v>3159</v>
       </c>
       <c r="BF389" s="70"/>
     </row>
@@ -75495,16 +75449,16 @@
         <v>43809</v>
       </c>
       <c r="C390" s="70">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D390" s="84" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="E390" s="70" t="s">
         <v>782</v>
       </c>
       <c r="F390" s="70" t="s">
-        <v>2464</v>
+        <v>1863</v>
       </c>
       <c r="G390" s="70" t="s">
         <v>1865</v>
@@ -75639,7 +75593,7 @@
         <v>2317</v>
       </c>
       <c r="AY390" s="70" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="AZ390" s="70" t="s">
         <v>941</v>
@@ -75651,50 +75605,50 @@
         <v>941</v>
       </c>
       <c r="BC390" s="70">
-        <v>35030</v>
+        <v>35028</v>
       </c>
       <c r="BD390" s="70">
-        <v>35030</v>
+        <v>35028</v>
       </c>
       <c r="BE390" s="70" t="s">
-        <v>3162</v>
+        <v>3160</v>
       </c>
       <c r="BF390" s="70"/>
     </row>
     <row r="391" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A391" s="70"/>
       <c r="B391" s="71">
-        <v>44229</v>
+        <v>43809</v>
       </c>
       <c r="C391" s="70">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D391" s="84" t="s">
-        <v>3464</v>
+        <v>1838</v>
       </c>
       <c r="E391" s="70" t="s">
         <v>782</v>
       </c>
       <c r="F391" s="70" t="s">
-        <v>3474</v>
+        <v>1864</v>
       </c>
       <c r="G391" s="70" t="s">
         <v>1865</v>
       </c>
       <c r="H391" s="75" t="s">
-        <v>3472</v>
+        <v>2463</v>
       </c>
       <c r="I391" s="70" t="s">
-        <v>3353</v>
+        <v>1417</v>
       </c>
       <c r="J391" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="K391" s="72" t="s">
-        <v>2319</v>
-      </c>
-      <c r="L391" s="72">
-        <v>70</v>
+      <c r="K391" s="72">
+        <v>60</v>
+      </c>
+      <c r="L391" s="72" t="s">
+        <v>2318</v>
       </c>
       <c r="M391" s="72">
         <v>0</v>
@@ -75703,30 +75657,74 @@
         <v>0</v>
       </c>
       <c r="O391" s="76" t="s">
-        <v>3468</v>
-      </c>
-      <c r="P391" s="76"/>
-      <c r="Q391" s="76"/>
-      <c r="R391" s="76"/>
-      <c r="S391" s="76"/>
-      <c r="T391" s="76"/>
-      <c r="U391" s="76"/>
-      <c r="V391" s="76"/>
-      <c r="W391" s="76"/>
-      <c r="X391" s="76"/>
-      <c r="Y391" s="76"/>
-      <c r="Z391" s="76"/>
-      <c r="AA391" s="76"/>
-      <c r="AB391" s="76"/>
-      <c r="AC391" s="76"/>
-      <c r="AD391" s="76"/>
-      <c r="AE391" s="70"/>
-      <c r="AF391" s="76"/>
-      <c r="AG391" s="76"/>
-      <c r="AH391" s="76"/>
-      <c r="AI391" s="76"/>
-      <c r="AJ391" s="76"/>
-      <c r="AK391" s="76"/>
+        <v>1867</v>
+      </c>
+      <c r="P391" s="76" t="s">
+        <v>1868</v>
+      </c>
+      <c r="Q391" s="76" t="s">
+        <v>1869</v>
+      </c>
+      <c r="R391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="S391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="T391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="U391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="V391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="W391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="X391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="Y391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="Z391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AA391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AB391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AC391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AD391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AE391" s="70" t="s">
+        <v>2263</v>
+      </c>
+      <c r="AF391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AG391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AH391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AI391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AJ391" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AK391" s="76" t="s">
+        <v>3178</v>
+      </c>
       <c r="AL391" s="70" t="s">
         <v>1870</v>
       </c>
@@ -75767,7 +75765,7 @@
         <v>2317</v>
       </c>
       <c r="AY391" s="70" t="s">
-        <v>3475</v>
+        <v>2849</v>
       </c>
       <c r="AZ391" s="70" t="s">
         <v>941</v>
@@ -75779,238 +75777,544 @@
         <v>941</v>
       </c>
       <c r="BC391" s="70">
-        <v>35031</v>
+        <v>35029</v>
       </c>
       <c r="BD391" s="70">
-        <v>35031</v>
+        <v>35029</v>
       </c>
       <c r="BE391" s="70" t="s">
-        <v>3477</v>
+        <v>3161</v>
       </c>
       <c r="BF391" s="70"/>
     </row>
-    <row r="392" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A392" s="70" t="s">
-        <v>1840</v>
-      </c>
-      <c r="B392" s="71"/>
-      <c r="C392" s="70"/>
-      <c r="D392" s="84"/>
-      <c r="E392" s="70"/>
-      <c r="F392" s="70"/>
-      <c r="G392" s="70"/>
-      <c r="H392" s="73"/>
-      <c r="I392" s="70"/>
-      <c r="J392" s="70"/>
-      <c r="K392" s="72"/>
-      <c r="L392" s="72"/>
-      <c r="M392" s="72"/>
-      <c r="N392" s="72"/>
-      <c r="O392" s="72"/>
-      <c r="P392" s="72"/>
-      <c r="Q392" s="72"/>
-      <c r="R392" s="72"/>
-      <c r="S392" s="72"/>
-      <c r="T392" s="72"/>
-      <c r="U392" s="70"/>
-      <c r="V392" s="70"/>
-      <c r="W392" s="70"/>
-      <c r="X392" s="70"/>
-      <c r="Y392" s="70"/>
-      <c r="Z392" s="70"/>
-      <c r="AA392" s="70"/>
-      <c r="AB392" s="70"/>
-      <c r="AC392" s="74"/>
-      <c r="AD392" s="74"/>
-      <c r="AE392" s="70"/>
-      <c r="AF392" s="70"/>
-      <c r="AG392" s="70"/>
-      <c r="AH392" s="70"/>
-      <c r="AI392" s="70"/>
-      <c r="AJ392" s="70"/>
-      <c r="AK392" s="70"/>
-      <c r="AL392" s="70"/>
-      <c r="AM392" s="70"/>
-      <c r="AN392" s="70"/>
-      <c r="AO392" s="70"/>
-      <c r="AP392" s="70"/>
-      <c r="AQ392" s="70"/>
-      <c r="AR392" s="70"/>
-      <c r="AS392" s="70"/>
-      <c r="AT392" s="70"/>
-      <c r="AU392" s="70"/>
-      <c r="AV392" s="70"/>
-      <c r="AW392" s="70"/>
-      <c r="AX392" s="70"/>
-      <c r="AY392" s="70"/>
-      <c r="AZ392" s="70"/>
-      <c r="BA392" s="70"/>
-      <c r="BB392" s="70"/>
-      <c r="BC392" s="70"/>
-      <c r="BD392" s="70"/>
-      <c r="BE392" s="70"/>
+    <row r="392" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A392" s="70"/>
+      <c r="B392" s="71">
+        <v>43809</v>
+      </c>
+      <c r="C392" s="70">
+        <v>30</v>
+      </c>
+      <c r="D392" s="84" t="s">
+        <v>1839</v>
+      </c>
+      <c r="E392" s="70" t="s">
+        <v>782</v>
+      </c>
+      <c r="F392" s="70" t="s">
+        <v>2464</v>
+      </c>
+      <c r="G392" s="70" t="s">
+        <v>1865</v>
+      </c>
+      <c r="H392" s="75" t="s">
+        <v>2463</v>
+      </c>
+      <c r="I392" s="70" t="s">
+        <v>1417</v>
+      </c>
+      <c r="J392" s="70" t="s">
+        <v>75</v>
+      </c>
+      <c r="K392" s="72">
+        <v>60</v>
+      </c>
+      <c r="L392" s="72" t="s">
+        <v>2318</v>
+      </c>
+      <c r="M392" s="72">
+        <v>0</v>
+      </c>
+      <c r="N392" s="72">
+        <v>0</v>
+      </c>
+      <c r="O392" s="76" t="s">
+        <v>1867</v>
+      </c>
+      <c r="P392" s="76" t="s">
+        <v>1868</v>
+      </c>
+      <c r="Q392" s="76" t="s">
+        <v>1869</v>
+      </c>
+      <c r="R392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="S392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="T392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="U392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="V392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="W392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="X392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="Y392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="Z392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AA392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AB392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AC392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AD392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AE392" s="70" t="s">
+        <v>2263</v>
+      </c>
+      <c r="AF392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AG392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AH392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AI392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AJ392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AK392" s="76" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AL392" s="70" t="s">
+        <v>1870</v>
+      </c>
+      <c r="AM392" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AN392" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AO392" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AP392" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AQ392" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AR392" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AS392" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AT392" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AU392" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AV392" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AW392" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AX392" s="70" t="s">
+        <v>2317</v>
+      </c>
+      <c r="AY392" s="70" t="s">
+        <v>2850</v>
+      </c>
+      <c r="AZ392" s="70" t="s">
+        <v>941</v>
+      </c>
+      <c r="BA392" s="70" t="s">
+        <v>941</v>
+      </c>
+      <c r="BB392" s="70" t="s">
+        <v>941</v>
+      </c>
+      <c r="BC392" s="70">
+        <v>35030</v>
+      </c>
+      <c r="BD392" s="70">
+        <v>35030</v>
+      </c>
+      <c r="BE392" s="70" t="s">
+        <v>3162</v>
+      </c>
       <c r="BF392" s="70"/>
     </row>
-    <row r="393" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A393" s="56" t="s">
+    <row r="393" spans="1:58" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A393" s="70"/>
+      <c r="B393" s="71">
+        <v>44229</v>
+      </c>
+      <c r="C393" s="70">
+        <v>31</v>
+      </c>
+      <c r="D393" s="84" t="s">
+        <v>3464</v>
+      </c>
+      <c r="E393" s="70" t="s">
+        <v>782</v>
+      </c>
+      <c r="F393" s="70" t="s">
+        <v>3474</v>
+      </c>
+      <c r="G393" s="70" t="s">
+        <v>1865</v>
+      </c>
+      <c r="H393" s="75" t="s">
+        <v>3472</v>
+      </c>
+      <c r="I393" s="70" t="s">
+        <v>3353</v>
+      </c>
+      <c r="J393" s="70" t="s">
+        <v>75</v>
+      </c>
+      <c r="K393" s="72" t="s">
+        <v>2319</v>
+      </c>
+      <c r="L393" s="72">
+        <v>70</v>
+      </c>
+      <c r="M393" s="72">
+        <v>0</v>
+      </c>
+      <c r="N393" s="72">
+        <v>0</v>
+      </c>
+      <c r="O393" s="76" t="s">
+        <v>3468</v>
+      </c>
+      <c r="P393" s="76"/>
+      <c r="Q393" s="76"/>
+      <c r="R393" s="76"/>
+      <c r="S393" s="76"/>
+      <c r="T393" s="76"/>
+      <c r="U393" s="76"/>
+      <c r="V393" s="76"/>
+      <c r="W393" s="76"/>
+      <c r="X393" s="76"/>
+      <c r="Y393" s="76"/>
+      <c r="Z393" s="76"/>
+      <c r="AA393" s="76"/>
+      <c r="AB393" s="76"/>
+      <c r="AC393" s="76"/>
+      <c r="AD393" s="76"/>
+      <c r="AE393" s="70"/>
+      <c r="AF393" s="76"/>
+      <c r="AG393" s="76"/>
+      <c r="AH393" s="76"/>
+      <c r="AI393" s="76"/>
+      <c r="AJ393" s="76"/>
+      <c r="AK393" s="76"/>
+      <c r="AL393" s="70" t="s">
+        <v>1870</v>
+      </c>
+      <c r="AM393" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AN393" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AO393" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AP393" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AQ393" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AR393" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AS393" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AT393" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AU393" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AV393" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AW393" s="70" t="s">
+        <v>888</v>
+      </c>
+      <c r="AX393" s="70" t="s">
+        <v>2317</v>
+      </c>
+      <c r="AY393" s="70" t="s">
+        <v>3475</v>
+      </c>
+      <c r="AZ393" s="70" t="s">
+        <v>941</v>
+      </c>
+      <c r="BA393" s="70" t="s">
+        <v>941</v>
+      </c>
+      <c r="BB393" s="70" t="s">
+        <v>941</v>
+      </c>
+      <c r="BC393" s="70">
+        <v>35031</v>
+      </c>
+      <c r="BD393" s="70">
+        <v>35031</v>
+      </c>
+      <c r="BE393" s="70" t="s">
+        <v>3477</v>
+      </c>
+      <c r="BF393" s="70"/>
+    </row>
+    <row r="394" spans="1:58" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A394" s="70" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B394" s="71"/>
+      <c r="C394" s="70"/>
+      <c r="D394" s="84"/>
+      <c r="E394" s="70"/>
+      <c r="F394" s="70"/>
+      <c r="G394" s="70"/>
+      <c r="H394" s="73"/>
+      <c r="I394" s="70"/>
+      <c r="J394" s="70"/>
+      <c r="K394" s="72"/>
+      <c r="L394" s="72"/>
+      <c r="M394" s="72"/>
+      <c r="N394" s="72"/>
+      <c r="O394" s="72"/>
+      <c r="P394" s="72"/>
+      <c r="Q394" s="72"/>
+      <c r="R394" s="72"/>
+      <c r="S394" s="72"/>
+      <c r="T394" s="72"/>
+      <c r="U394" s="70"/>
+      <c r="V394" s="70"/>
+      <c r="W394" s="70"/>
+      <c r="X394" s="70"/>
+      <c r="Y394" s="70"/>
+      <c r="Z394" s="70"/>
+      <c r="AA394" s="70"/>
+      <c r="AB394" s="70"/>
+      <c r="AC394" s="74"/>
+      <c r="AD394" s="74"/>
+      <c r="AE394" s="70"/>
+      <c r="AF394" s="70"/>
+      <c r="AG394" s="70"/>
+      <c r="AH394" s="70"/>
+      <c r="AI394" s="70"/>
+      <c r="AJ394" s="70"/>
+      <c r="AK394" s="70"/>
+      <c r="AL394" s="70"/>
+      <c r="AM394" s="70"/>
+      <c r="AN394" s="70"/>
+      <c r="AO394" s="70"/>
+      <c r="AP394" s="70"/>
+      <c r="AQ394" s="70"/>
+      <c r="AR394" s="70"/>
+      <c r="AS394" s="70"/>
+      <c r="AT394" s="70"/>
+      <c r="AU394" s="70"/>
+      <c r="AV394" s="70"/>
+      <c r="AW394" s="70"/>
+      <c r="AX394" s="70"/>
+      <c r="AY394" s="70"/>
+      <c r="AZ394" s="70"/>
+      <c r="BA394" s="70"/>
+      <c r="BB394" s="70"/>
+      <c r="BC394" s="70"/>
+      <c r="BD394" s="70"/>
+      <c r="BE394" s="70"/>
+      <c r="BF394" s="70"/>
+    </row>
+    <row r="395" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A395" s="56" t="s">
         <v>832</v>
       </c>
-      <c r="B393" s="57"/>
-      <c r="C393" s="56"/>
-      <c r="D393" s="85"/>
-      <c r="E393" s="56"/>
-      <c r="F393" s="56"/>
-      <c r="G393" s="56"/>
-      <c r="H393" s="58"/>
-      <c r="I393" s="56"/>
-      <c r="J393" s="56"/>
-      <c r="K393" s="56"/>
-      <c r="L393" s="56"/>
-      <c r="M393" s="56"/>
-      <c r="N393" s="56"/>
-      <c r="O393" s="56"/>
-      <c r="P393" s="56"/>
-      <c r="Q393" s="56"/>
-      <c r="R393" s="56"/>
-      <c r="S393" s="56"/>
-      <c r="T393" s="56"/>
-      <c r="U393" s="56"/>
-      <c r="V393" s="56"/>
-      <c r="W393" s="56"/>
-      <c r="X393" s="56"/>
-      <c r="Y393" s="56"/>
-      <c r="Z393" s="56"/>
-      <c r="AA393" s="56"/>
-      <c r="AB393" s="56"/>
-      <c r="AC393" s="56"/>
-      <c r="AD393" s="56"/>
-      <c r="AE393" s="56"/>
-      <c r="AF393" s="56"/>
-      <c r="AG393" s="56"/>
-      <c r="AH393" s="56"/>
-      <c r="AI393" s="56"/>
-      <c r="AJ393" s="56"/>
-      <c r="AK393" s="56"/>
-      <c r="AL393" s="56"/>
-      <c r="AM393" s="56"/>
-      <c r="AN393" s="56"/>
-      <c r="AO393" s="56"/>
-      <c r="AP393" s="56"/>
-      <c r="AQ393" s="56"/>
-      <c r="AR393" s="56"/>
-      <c r="AS393" s="56"/>
-      <c r="AT393" s="56"/>
-      <c r="AU393" s="56"/>
-      <c r="AV393" s="56"/>
-      <c r="AW393" s="56"/>
-      <c r="AX393" s="56"/>
-      <c r="AY393" s="56"/>
-      <c r="AZ393" s="56"/>
-      <c r="BA393" s="56"/>
-      <c r="BB393" s="56"/>
-      <c r="BC393" s="56"/>
-      <c r="BD393" s="56"/>
-      <c r="BE393" s="56"/>
-      <c r="BF393" s="56"/>
+      <c r="B395" s="57"/>
+      <c r="C395" s="56"/>
+      <c r="D395" s="85"/>
+      <c r="E395" s="56"/>
+      <c r="F395" s="56"/>
+      <c r="G395" s="56"/>
+      <c r="H395" s="58"/>
+      <c r="I395" s="56"/>
+      <c r="J395" s="56"/>
+      <c r="K395" s="56"/>
+      <c r="L395" s="56"/>
+      <c r="M395" s="56"/>
+      <c r="N395" s="56"/>
+      <c r="O395" s="56"/>
+      <c r="P395" s="56"/>
+      <c r="Q395" s="56"/>
+      <c r="R395" s="56"/>
+      <c r="S395" s="56"/>
+      <c r="T395" s="56"/>
+      <c r="U395" s="56"/>
+      <c r="V395" s="56"/>
+      <c r="W395" s="56"/>
+      <c r="X395" s="56"/>
+      <c r="Y395" s="56"/>
+      <c r="Z395" s="56"/>
+      <c r="AA395" s="56"/>
+      <c r="AB395" s="56"/>
+      <c r="AC395" s="56"/>
+      <c r="AD395" s="56"/>
+      <c r="AE395" s="56"/>
+      <c r="AF395" s="56"/>
+      <c r="AG395" s="56"/>
+      <c r="AH395" s="56"/>
+      <c r="AI395" s="56"/>
+      <c r="AJ395" s="56"/>
+      <c r="AK395" s="56"/>
+      <c r="AL395" s="56"/>
+      <c r="AM395" s="56"/>
+      <c r="AN395" s="56"/>
+      <c r="AO395" s="56"/>
+      <c r="AP395" s="56"/>
+      <c r="AQ395" s="56"/>
+      <c r="AR395" s="56"/>
+      <c r="AS395" s="56"/>
+      <c r="AT395" s="56"/>
+      <c r="AU395" s="56"/>
+      <c r="AV395" s="56"/>
+      <c r="AW395" s="56"/>
+      <c r="AX395" s="56"/>
+      <c r="AY395" s="56"/>
+      <c r="AZ395" s="56"/>
+      <c r="BA395" s="56"/>
+      <c r="BB395" s="56"/>
+      <c r="BC395" s="56"/>
+      <c r="BD395" s="56"/>
+      <c r="BE395" s="56"/>
+      <c r="BF395" s="56"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BF393" xr:uid="{A6EE1CE3-DC85-4AC8-ADB1-E8F1B02F8C62}"/>
+  <autoFilter ref="A1:BF395" xr:uid="{A6EE1CE3-DC85-4AC8-ADB1-E8F1B02F8C62}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="F281">
-    <cfRule type="duplicateValues" dxfId="31" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F346 F328">
-    <cfRule type="duplicateValues" dxfId="30" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F375">
-    <cfRule type="duplicateValues" dxfId="29" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F347">
+    <cfRule type="duplicateValues" dxfId="30" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F348:F355">
+    <cfRule type="duplicateValues" dxfId="29" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F100">
     <cfRule type="duplicateValues" dxfId="28" priority="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F348:F355">
+  <conditionalFormatting sqref="F86:F99">
     <cfRule type="duplicateValues" dxfId="27" priority="31"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F100">
+  <conditionalFormatting sqref="F194">
     <cfRule type="duplicateValues" dxfId="26" priority="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F86:F99">
+  <conditionalFormatting sqref="F287">
     <cfRule type="duplicateValues" dxfId="25" priority="29"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F194">
+  <conditionalFormatting sqref="F394 F300:F312 F387:F391">
     <cfRule type="duplicateValues" dxfId="24" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F287">
+  <conditionalFormatting sqref="F284:F286">
     <cfRule type="duplicateValues" dxfId="23" priority="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F392 F300:F312 F385:F389">
+  <conditionalFormatting sqref="F193">
     <cfRule type="duplicateValues" dxfId="22" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F284:F286">
+  <conditionalFormatting sqref="F356:F374">
     <cfRule type="duplicateValues" dxfId="21" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F193">
-    <cfRule type="duplicateValues" dxfId="20" priority="24"/>
+  <conditionalFormatting sqref="F322:F326">
+    <cfRule type="duplicateValues" dxfId="20" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F356:F374">
-    <cfRule type="duplicateValues" dxfId="19" priority="23"/>
+  <conditionalFormatting sqref="F377">
+    <cfRule type="duplicateValues" dxfId="19" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F322:F326">
+  <conditionalFormatting sqref="F2">
     <cfRule type="duplicateValues" dxfId="18" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F377">
+  <conditionalFormatting sqref="F288:F299">
     <cfRule type="duplicateValues" dxfId="17" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2">
+  <conditionalFormatting sqref="F392:F393">
     <cfRule type="duplicateValues" dxfId="16" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F288:F299">
-    <cfRule type="duplicateValues" dxfId="15" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F390:F391">
-    <cfRule type="duplicateValues" dxfId="14" priority="17"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F313">
-    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F163:F182">
-    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O378:O379">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O369">
+    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O342:O343">
+    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O386">
     <cfRule type="duplicateValues" dxfId="10" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O342:O343">
-    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
+  <conditionalFormatting sqref="O379:O381 O384">
+    <cfRule type="duplicateValues" dxfId="9" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O384">
     <cfRule type="duplicateValues" dxfId="8" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O379:O382">
-    <cfRule type="duplicateValues" dxfId="7" priority="55"/>
+  <conditionalFormatting sqref="O381">
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O382">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+  <conditionalFormatting sqref="F395:F1048576 F1 F327 F3:F85 F101:F162 F195:F280 F282:F283 F314:F321 F183:F192">
+    <cfRule type="duplicateValues" dxfId="6" priority="67"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O381">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F393:F1048576 F1 F327 F3:F85 F101:F162 F195:F280 F282:F283 F314:F321 F183:F192">
-    <cfRule type="duplicateValues" dxfId="4" priority="65"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O385:O1048576 O346:O368 O383 O370:O377 O1:O340">
-    <cfRule type="duplicateValues" dxfId="3" priority="75"/>
+  <conditionalFormatting sqref="O387:O1048576 O346:O368 O385 O370:O377 O1:O340">
+    <cfRule type="duplicateValues" dxfId="5" priority="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O345">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O341">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O344">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O341">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="O382:O383">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O344">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="O383">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
remove old pvp. fix unreal ultima
</commit_message>
<xml_diff>
--- a/guide_ffxiv.xlsx
+++ b/guide_ffxiv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Github\DevFFXIVPocketGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B38D15B-C56F-4A2E-8E59-9554608CD324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0559C565-9860-4E2C-BD28-7FB7712320C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3015" yWindow="4200" windowWidth="31230" windowHeight="15435" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
   </bookViews>
@@ -11289,10 +11289,10 @@
   <dimension ref="A1:AS456"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AJ377" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E426" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL410" sqref="AL410"/>
+      <selection pane="bottomRight" activeCell="A446" sqref="A446:F446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -11313,25 +11313,25 @@
     <col min="14" max="14" width="11.42578125" style="1" customWidth="1" outlineLevel="1"/>
     <col min="15" max="15" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="39.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="31.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="19.28515625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="58.5703125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="33" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="38.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="36.140625" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="24.42578125" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="24" max="24" width="27.140625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="26" width="23.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.28515625" style="1" hidden="1" customWidth="1" outlineLevel="2" collapsed="1"/>
-    <col min="28" max="28" width="14.5703125" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="29" max="29" width="14.85546875" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="12.28515625" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="31" max="31" width="18.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="10.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="28.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="17" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="11.140625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="31.7109375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="19.28515625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="58.5703125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="33" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="38.7109375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="36.140625" style="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="24.42578125" style="1" customWidth="1" outlineLevel="2"/>
+    <col min="24" max="24" width="27.140625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="26" width="23.7109375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.28515625" style="1" customWidth="1" outlineLevel="2" collapsed="1"/>
+    <col min="28" max="28" width="14.5703125" style="1" customWidth="1" outlineLevel="2"/>
+    <col min="29" max="29" width="14.85546875" style="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="12.28515625" style="1" customWidth="1" outlineLevel="2"/>
+    <col min="31" max="31" width="18.85546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="10.7109375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="28.85546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="17" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="11.140625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="56.140625" style="1" customWidth="1"/>
     <col min="39" max="39" width="8" style="1" bestFit="1" customWidth="1"/>
@@ -63092,7 +63092,7 @@
         <v>3344</v>
       </c>
       <c r="AL411" s="87" t="s">
-        <v>925</v>
+        <v>1146</v>
       </c>
       <c r="AM411" s="87" t="s">
         <v>925</v>
@@ -63185,7 +63185,7 @@
         <v>3349</v>
       </c>
       <c r="AL412" s="87" t="s">
-        <v>925</v>
+        <v>1146</v>
       </c>
       <c r="AM412" s="87" t="s">
         <v>925</v>

</xml_diff>

<commit_message>
readded major part after fixing most stuff
</commit_message>
<xml_diff>
--- a/guide_ffxiv.xlsx
+++ b/guide_ffxiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Github\DevFFXIVPocketGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB621E96-8627-4E7C-B136-5450069F7C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD68F895-2701-4274-AA42-4B9D3ECDB902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39180" yWindow="780" windowWidth="38700" windowHeight="15435" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="35730" windowHeight="15435" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14036" uniqueCount="3397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14034" uniqueCount="3397">
   <si>
     <t>date:</t>
   </si>
@@ -11326,14 +11326,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB88280F-F23E-48B4-9B91-E7EC59D48F52}">
-  <sheetPr codeName="Tabelle1"/>
+  <sheetPr codeName="Tabelle1" filterMode="1"/>
   <dimension ref="A1:AS456"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AH373" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AK380" sqref="AK380"/>
+      <selection pane="bottomRight" activeCell="AS84" sqref="AS84:AS376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -15776,7 +15776,7 @@
       </c>
       <c r="AS33" s="6"/>
     </row>
-    <row r="34" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>766</v>
       </c>
@@ -19418,7 +19418,7 @@
       </c>
       <c r="AS61" s="6"/>
     </row>
-    <row r="62" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>769</v>
       </c>
@@ -22128,7 +22128,7 @@
       </c>
       <c r="AS82" s="6"/>
     </row>
-    <row r="83" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>772</v>
       </c>
@@ -22177,7 +22177,7 @@
       <c r="AR83" s="6"/>
       <c r="AS83" s="6"/>
     </row>
-    <row r="84" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="7">
         <v>41828</v>
@@ -22302,7 +22302,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="85" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>776</v>
       </c>
@@ -24213,7 +24213,7 @@
       </c>
       <c r="AS99" s="6"/>
     </row>
-    <row r="100" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>1951</v>
       </c>
@@ -26656,7 +26656,7 @@
       </c>
       <c r="AS118" s="14"/>
     </row>
-    <row r="119" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
         <v>767</v>
       </c>
@@ -28568,7 +28568,7 @@
       </c>
       <c r="AS133" s="14"/>
     </row>
-    <row r="134" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
         <v>770</v>
       </c>
@@ -32208,7 +32208,7 @@
       </c>
       <c r="AS161" s="14"/>
     </row>
-    <row r="162" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
         <v>773</v>
       </c>
@@ -34917,7 +34917,7 @@
       </c>
       <c r="AS182" s="14"/>
     </row>
-    <row r="183" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
         <v>2049</v>
       </c>
@@ -34966,7 +34966,7 @@
       <c r="AR183" s="14"/>
       <c r="AS183" s="14"/>
     </row>
-    <row r="184" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A184" s="14"/>
       <c r="B184" s="15">
         <v>42206</v>
@@ -35101,7 +35101,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="185" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A185" s="14"/>
       <c r="B185" s="15">
         <v>42458</v>
@@ -35234,7 +35234,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="186" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A186" s="14"/>
       <c r="B186" s="15">
         <v>42458</v>
@@ -35367,7 +35367,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="187" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A187" s="14"/>
       <c r="B187" s="15">
         <v>42528</v>
@@ -35502,7 +35502,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="188" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A188" s="14"/>
       <c r="B188" s="15">
         <v>42640</v>
@@ -35635,7 +35635,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="189" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" s="14"/>
       <c r="B189" s="15">
         <v>42794</v>
@@ -35768,7 +35768,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="190" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A190" s="14"/>
       <c r="B190" s="15">
         <v>42794</v>
@@ -35901,7 +35901,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="191" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" s="14"/>
       <c r="B191" s="15">
         <v>42794</v>
@@ -36034,7 +36034,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="192" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="14" t="s">
         <v>777</v>
       </c>
@@ -36180,7 +36180,7 @@
       </c>
       <c r="AS193" s="14"/>
     </row>
-    <row r="194" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A194" s="14" t="s">
         <v>1387</v>
       </c>
@@ -38224,7 +38224,7 @@
       </c>
       <c r="AS209" s="20"/>
     </row>
-    <row r="210" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A210" s="20" t="s">
         <v>768</v>
       </c>
@@ -40534,7 +40534,7 @@
       </c>
       <c r="AS227" s="20"/>
     </row>
-    <row r="228" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A228" s="20" t="s">
         <v>771</v>
       </c>
@@ -44441,7 +44441,7 @@
       </c>
       <c r="AS257" s="20"/>
     </row>
-    <row r="258" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A258" s="20" t="s">
         <v>774</v>
       </c>
@@ -45820,7 +45820,7 @@
       </c>
       <c r="AS268" s="20"/>
     </row>
-    <row r="269" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A269" s="20" t="s">
         <v>775</v>
       </c>
@@ -45869,7 +45869,7 @@
       <c r="AR269" s="20"/>
       <c r="AS269" s="20"/>
     </row>
-    <row r="270" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A270" s="20"/>
       <c r="B270" s="21">
         <v>43060</v>
@@ -46004,7 +46004,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="271" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A271" s="20"/>
       <c r="B271" s="21">
         <v>43130</v>
@@ -46137,7 +46137,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="272" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A272" s="20"/>
       <c r="B272" s="21">
         <v>43130</v>
@@ -46270,7 +46270,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="273" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A273" s="20"/>
       <c r="B273" s="21">
         <v>43130</v>
@@ -46403,7 +46403,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="274" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A274" s="20"/>
       <c r="B274" s="21">
         <v>43130</v>
@@ -46536,7 +46536,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="275" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A275" s="20"/>
       <c r="B275" s="21">
         <v>43130</v>
@@ -46669,7 +46669,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="276" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A276" s="20"/>
       <c r="B276" s="21">
         <v>43477</v>
@@ -46804,7 +46804,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="277" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="20" t="s">
         <v>778</v>
       </c>
@@ -47309,7 +47309,7 @@
       </c>
       <c r="AS281" s="20"/>
     </row>
-    <row r="282" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A282" s="20"/>
       <c r="B282" s="21">
         <v>43477</v>
@@ -47420,7 +47420,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="283" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="20" t="s">
         <v>2299</v>
       </c>
@@ -47760,7 +47760,7 @@
       </c>
       <c r="AS286" s="20"/>
     </row>
-    <row r="287" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A287" s="20" t="s">
         <v>1388</v>
       </c>
@@ -51134,7 +51134,7 @@
       </c>
       <c r="AS312" s="70"/>
     </row>
-    <row r="313" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A313" s="70" t="s">
         <v>1486</v>
       </c>
@@ -52912,7 +52912,7 @@
       </c>
       <c r="AS326" s="28"/>
     </row>
-    <row r="327" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A327" s="28" t="s">
         <v>779</v>
       </c>
@@ -54422,7 +54422,7 @@
       </c>
       <c r="AS338" s="28"/>
     </row>
-    <row r="339" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A339" s="28"/>
       <c r="B339" s="38">
         <v>44054</v>
@@ -54553,9 +54553,7 @@
       <c r="AR339" s="28" t="s">
         <v>2509</v>
       </c>
-      <c r="AS339" s="28" t="s">
-        <v>2074</v>
-      </c>
+      <c r="AS339" s="28"/>
     </row>
     <row r="340" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A340" s="28"/>
@@ -54823,7 +54821,7 @@
       </c>
       <c r="AS341" s="28"/>
     </row>
-    <row r="342" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A342" s="28"/>
       <c r="B342" s="38">
         <v>44173</v>
@@ -54954,9 +54952,7 @@
       <c r="AR342" s="28" t="s">
         <v>2942</v>
       </c>
-      <c r="AS342" s="28" t="s">
-        <v>2074</v>
-      </c>
+      <c r="AS342" s="28"/>
     </row>
     <row r="343" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A343" s="28"/>
@@ -55349,7 +55345,7 @@
       </c>
       <c r="AS345" s="28"/>
     </row>
-    <row r="346" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="28" t="s">
         <v>780</v>
       </c>
@@ -55398,7 +55394,7 @@
       <c r="AR346" s="28"/>
       <c r="AS346" s="28"/>
     </row>
-    <row r="347" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A347" s="28"/>
       <c r="B347" s="35">
         <v>43767</v>
@@ -55531,7 +55527,7 @@
       </c>
       <c r="AS347" s="28"/>
     </row>
-    <row r="348" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A348" s="28"/>
       <c r="B348" s="35">
         <v>44054</v>
@@ -55664,7 +55660,7 @@
       </c>
       <c r="AS348" s="28"/>
     </row>
-    <row r="349" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A349" s="28"/>
       <c r="B349" s="29">
         <v>44299</v>
@@ -55797,7 +55793,7 @@
       </c>
       <c r="AS349" s="28"/>
     </row>
-    <row r="350" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A350" s="28"/>
       <c r="B350" s="35">
         <v>43662</v>
@@ -55930,7 +55926,7 @@
       </c>
       <c r="AS350" s="28"/>
     </row>
-    <row r="351" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A351" s="28"/>
       <c r="B351" s="35">
         <v>43662</v>
@@ -56063,7 +56059,7 @@
       </c>
       <c r="AS351" s="28"/>
     </row>
-    <row r="352" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A352" s="28"/>
       <c r="B352" s="35">
         <v>43662</v>
@@ -56196,7 +56192,7 @@
       </c>
       <c r="AS352" s="28"/>
     </row>
-    <row r="353" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A353" s="28"/>
       <c r="B353" s="35">
         <v>43662</v>
@@ -56329,7 +56325,7 @@
       </c>
       <c r="AS353" s="28"/>
     </row>
-    <row r="354" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A354" s="28"/>
       <c r="B354" s="35">
         <v>43676</v>
@@ -56462,7 +56458,7 @@
       </c>
       <c r="AS354" s="28"/>
     </row>
-    <row r="355" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A355" s="28"/>
       <c r="B355" s="35">
         <v>43676</v>
@@ -56595,7 +56591,7 @@
       </c>
       <c r="AS355" s="28"/>
     </row>
-    <row r="356" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A356" s="28"/>
       <c r="B356" s="35">
         <v>43676</v>
@@ -56728,7 +56724,7 @@
       </c>
       <c r="AS356" s="28"/>
     </row>
-    <row r="357" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A357" s="28"/>
       <c r="B357" s="35">
         <v>43676</v>
@@ -56861,7 +56857,7 @@
       </c>
       <c r="AS357" s="28"/>
     </row>
-    <row r="358" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A358" s="28"/>
       <c r="B358" s="35">
         <v>43848</v>
@@ -56994,7 +56990,7 @@
       </c>
       <c r="AS358" s="28"/>
     </row>
-    <row r="359" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A359" s="28"/>
       <c r="B359" s="35">
         <v>43848</v>
@@ -57127,7 +57123,7 @@
       </c>
       <c r="AS359" s="28"/>
     </row>
-    <row r="360" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A360" s="28"/>
       <c r="B360" s="35">
         <v>43848</v>
@@ -57260,7 +57256,7 @@
       </c>
       <c r="AS360" s="28"/>
     </row>
-    <row r="361" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A361" s="28"/>
       <c r="B361" s="35">
         <v>43848</v>
@@ -57393,7 +57389,7 @@
       </c>
       <c r="AS361" s="28"/>
     </row>
-    <row r="362" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A362" s="28"/>
       <c r="B362" s="35">
         <v>43848</v>
@@ -57526,7 +57522,7 @@
       </c>
       <c r="AS362" s="28"/>
     </row>
-    <row r="363" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A363" s="28"/>
       <c r="B363" s="35">
         <v>43848</v>
@@ -57659,7 +57655,7 @@
       </c>
       <c r="AS363" s="28"/>
     </row>
-    <row r="364" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A364" s="28"/>
       <c r="B364" s="35">
         <v>43848</v>
@@ -57792,7 +57788,7 @@
       </c>
       <c r="AS364" s="28"/>
     </row>
-    <row r="365" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A365" s="28"/>
       <c r="B365" s="35">
         <v>43848</v>
@@ -57925,7 +57921,7 @@
       </c>
       <c r="AS365" s="28"/>
     </row>
-    <row r="366" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A366" s="28"/>
       <c r="B366" s="35">
         <v>44173</v>
@@ -58056,7 +58052,7 @@
       </c>
       <c r="AS366" s="28"/>
     </row>
-    <row r="367" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A367" s="28"/>
       <c r="B367" s="35">
         <v>44173</v>
@@ -58189,7 +58185,7 @@
       </c>
       <c r="AS367" s="28"/>
     </row>
-    <row r="368" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A368" s="28"/>
       <c r="B368" s="35">
         <v>44173</v>
@@ -58322,7 +58318,7 @@
       </c>
       <c r="AS368" s="28"/>
     </row>
-    <row r="369" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A369" s="28"/>
       <c r="B369" s="35">
         <v>44173</v>
@@ -58455,7 +58451,7 @@
       </c>
       <c r="AS369" s="28"/>
     </row>
-    <row r="370" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A370" s="28"/>
       <c r="B370" s="35">
         <v>44173</v>
@@ -58588,7 +58584,7 @@
       </c>
       <c r="AS370" s="28"/>
     </row>
-    <row r="371" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A371" s="28"/>
       <c r="B371" s="35">
         <v>44173</v>
@@ -58721,7 +58717,7 @@
       </c>
       <c r="AS371" s="28"/>
     </row>
-    <row r="372" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A372" s="28"/>
       <c r="B372" s="35">
         <v>44173</v>
@@ -58854,7 +58850,7 @@
       </c>
       <c r="AS372" s="28"/>
     </row>
-    <row r="373" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A373" s="28"/>
       <c r="B373" s="35">
         <v>44173</v>
@@ -58987,7 +58983,7 @@
       </c>
       <c r="AS373" s="28"/>
     </row>
-    <row r="374" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A374" s="28"/>
       <c r="B374" s="35">
         <v>43781</v>
@@ -59120,7 +59116,7 @@
       </c>
       <c r="AS374" s="28"/>
     </row>
-    <row r="375" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A375" s="28" t="s">
         <v>781</v>
       </c>
@@ -59169,7 +59165,7 @@
       <c r="AR375" s="28"/>
       <c r="AS375" s="28"/>
     </row>
-    <row r="376" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A376" s="28"/>
       <c r="B376" s="35">
         <v>43809</v>
@@ -59302,7 +59298,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="377" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="28" t="s">
         <v>1411</v>
       </c>
@@ -59351,7 +59347,7 @@
       <c r="AR377" s="28"/>
       <c r="AS377" s="28"/>
     </row>
-    <row r="378" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A378" s="28"/>
       <c r="B378" s="35">
         <v>44117</v>
@@ -59480,7 +59476,7 @@
       </c>
       <c r="AS378" s="28"/>
     </row>
-    <row r="379" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A379" s="28"/>
       <c r="B379" s="35">
         <v>44117</v>
@@ -59609,7 +59605,7 @@
       </c>
       <c r="AS379" s="28"/>
     </row>
-    <row r="380" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A380" s="28"/>
       <c r="B380" s="35">
         <v>44229</v>
@@ -59728,7 +59724,7 @@
       </c>
       <c r="AS380" s="28"/>
     </row>
-    <row r="381" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A381" s="28"/>
       <c r="B381" s="35">
         <v>44229</v>
@@ -59847,7 +59843,7 @@
       </c>
       <c r="AS381" s="28"/>
     </row>
-    <row r="382" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A382" s="28"/>
       <c r="B382" s="35">
         <v>44117</v>
@@ -59936,7 +59932,7 @@
       </c>
       <c r="AS382" s="28"/>
     </row>
-    <row r="383" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A383" s="28"/>
       <c r="B383" s="35">
         <v>44117</v>
@@ -60027,7 +60023,7 @@
       </c>
       <c r="AS383" s="28"/>
     </row>
-    <row r="384" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A384" s="35" t="s">
         <v>3015</v>
       </c>
@@ -60264,7 +60260,7 @@
       </c>
       <c r="AS386" s="28"/>
     </row>
-    <row r="387" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A387" s="28" t="s">
         <v>1389</v>
       </c>
@@ -61071,7 +61067,7 @@
       </c>
       <c r="AS393" s="70"/>
     </row>
-    <row r="394" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A394" s="70" t="s">
         <v>1460</v>
       </c>
@@ -62277,7 +62273,7 @@
       </c>
       <c r="AS403" s="87"/>
     </row>
-    <row r="404" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A404" s="87" t="s">
         <v>3201</v>
       </c>
@@ -63250,7 +63246,7 @@
       </c>
       <c r="AS412" s="87"/>
     </row>
-    <row r="413" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A413" s="87" t="s">
         <v>3200</v>
       </c>
@@ -63299,7 +63295,7 @@
       <c r="AR413" s="87"/>
       <c r="AS413" s="87"/>
     </row>
-    <row r="414" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A414" s="87"/>
       <c r="B414" s="88">
         <v>44663</v>
@@ -63392,7 +63388,7 @@
       </c>
       <c r="AS414" s="87"/>
     </row>
-    <row r="415" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A415" s="87"/>
       <c r="B415" s="88">
         <v>44551</v>
@@ -63525,7 +63521,7 @@
       </c>
       <c r="AS415" s="87"/>
     </row>
-    <row r="416" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A416" s="87"/>
       <c r="B416" s="88">
         <v>44551</v>
@@ -63658,7 +63654,7 @@
       </c>
       <c r="AS416" s="87"/>
     </row>
-    <row r="417" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A417" s="87"/>
       <c r="B417" s="88">
         <v>44551</v>
@@ -63791,7 +63787,7 @@
       </c>
       <c r="AS417" s="87"/>
     </row>
-    <row r="418" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A418" s="87"/>
       <c r="B418" s="88">
         <v>44551</v>
@@ -63924,7 +63920,7 @@
       </c>
       <c r="AS418" s="87"/>
     </row>
-    <row r="419" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A419" s="87"/>
       <c r="B419" s="88">
         <v>44565</v>
@@ -64057,7 +64053,7 @@
       </c>
       <c r="AS419" s="87"/>
     </row>
-    <row r="420" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A420" s="87"/>
       <c r="B420" s="88">
         <v>44565</v>
@@ -64190,7 +64186,7 @@
       </c>
       <c r="AS420" s="87"/>
     </row>
-    <row r="421" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A421" s="87"/>
       <c r="B421" s="88">
         <v>44565</v>
@@ -64323,7 +64319,7 @@
       </c>
       <c r="AS421" s="87"/>
     </row>
-    <row r="422" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A422" s="87"/>
       <c r="B422" s="88">
         <v>44565</v>
@@ -64456,7 +64452,7 @@
       </c>
       <c r="AS422" s="87"/>
     </row>
-    <row r="423" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A423" s="87"/>
       <c r="B423" s="88">
         <v>44677</v>
@@ -64543,7 +64539,7 @@
       <c r="AR423" s="87"/>
       <c r="AS423" s="87"/>
     </row>
-    <row r="424" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A424" s="87" t="s">
         <v>3199</v>
       </c>
@@ -66977,7 +66973,7 @@
       <c r="AR451" s="87"/>
       <c r="AS451" s="87"/>
     </row>
-    <row r="452" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:45" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A452" s="87" t="s">
         <v>3204</v>
       </c>
@@ -67026,7 +67022,7 @@
       <c r="AR452" s="87"/>
       <c r="AS452" s="87"/>
     </row>
-    <row r="453" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" s="87"/>
       <c r="B453" s="88">
         <v>44565</v>
@@ -67157,7 +67153,7 @@
       </c>
       <c r="AS453" s="87"/>
     </row>
-    <row r="454" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" s="87" t="s">
         <v>3198</v>
       </c>
@@ -67206,7 +67202,7 @@
       <c r="AR454" s="87"/>
       <c r="AS454" s="87"/>
     </row>
-    <row r="455" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" s="56" t="s">
         <v>832</v>
       </c>
@@ -67259,7 +67255,13 @@
       <c r="H456" s="90"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AS455" xr:uid="{A6EE1CE3-DC85-4AC8-ADB1-E8F1B02F8C62}"/>
+  <autoFilter ref="A1:AS455" xr:uid="{A6EE1CE3-DC85-4AC8-ADB1-E8F1B02F8C62}">
+    <filterColumn colId="44">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="F281">
     <cfRule type="duplicateValues" dxfId="33" priority="41"/>

</xml_diff>

<commit_message>
fix names + color + difficulty
</commit_message>
<xml_diff>
--- a/guide_ffxiv.xlsx
+++ b/guide_ffxiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Github\DevFFXIVPocketGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F8D07C-7E86-4537-9928-5542FDBA63C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5C1821-C8B0-40D7-8EC8-040D8EC6EC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39180" yWindow="780" windowWidth="38700" windowHeight="15435" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
+    <workbookView xWindow="495" yWindow="1905" windowWidth="38700" windowHeight="15435" xr2:uid="{3F3FA391-F620-48D4-9F69-F3B9E653815F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14035" uniqueCount="3398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14034" uniqueCount="3397">
   <si>
     <t>date:</t>
   </si>
@@ -10100,9 +10100,6 @@
   </si>
   <si>
     <t>ui/icon/112000/112470.tex</t>
-  </si>
-  <si>
-    <t>Unreal</t>
   </si>
   <si>
     <t>w1fb_2</t>
@@ -11333,18 +11330,18 @@
   <dimension ref="A1:AS456"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AK228" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E330" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL424" sqref="AL424"/>
+      <selection pane="bottomRight" activeCell="I411" sqref="I411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="9" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="46.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="9" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="46.5703125" style="86" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="47.85546875" style="1" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="24.7109375" style="1" customWidth="1" outlineLevel="1"/>
@@ -11357,25 +11354,25 @@
     <col min="14" max="14" width="11.42578125" style="1" customWidth="1" outlineLevel="1"/>
     <col min="15" max="15" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="39.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="31.7109375" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="19.28515625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="58.5703125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="33" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="38.7109375" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="36.140625" style="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="24.42578125" style="1" customWidth="1" outlineLevel="2"/>
-    <col min="24" max="24" width="27.140625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="26" width="23.7109375" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.28515625" style="1" customWidth="1" outlineLevel="2" collapsed="1"/>
-    <col min="28" max="28" width="14.5703125" style="1" customWidth="1" outlineLevel="2"/>
-    <col min="29" max="29" width="14.85546875" style="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="12.28515625" style="1" customWidth="1" outlineLevel="2"/>
-    <col min="31" max="31" width="18.85546875" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="10.7109375" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="28.85546875" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="17" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="11.140625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="19.28515625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="58.5703125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="33" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="38.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="36.140625" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="24.42578125" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="24" max="24" width="27.140625" style="1" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="25" max="26" width="23.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.28515625" style="1" hidden="1" customWidth="1" outlineLevel="2" collapsed="1"/>
+    <col min="28" max="28" width="14.5703125" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="29" max="29" width="14.85546875" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="12.28515625" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="31" max="31" width="18.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="32" max="32" width="10.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="28.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="17" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="11.140625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="56.140625" style="1" customWidth="1"/>
     <col min="39" max="39" width="8" style="1" bestFit="1" customWidth="1"/>
@@ -16228,9 +16225,7 @@
       <c r="AS37" s="6"/>
     </row>
     <row r="38" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>3374</v>
-      </c>
+      <c r="A38" s="6"/>
       <c r="B38" s="7">
         <v>41513</v>
       </c>
@@ -52962,7 +52957,7 @@
       <c r="AR327" s="28"/>
       <c r="AS327" s="28"/>
     </row>
-    <row r="328" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A328" s="28"/>
       <c r="B328" s="38">
         <v>43644</v>
@@ -53095,7 +53090,7 @@
       </c>
       <c r="AS328" s="28"/>
     </row>
-    <row r="329" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A329" s="28"/>
       <c r="B329" s="38">
         <v>43644</v>
@@ -53228,7 +53223,7 @@
       </c>
       <c r="AS329" s="28"/>
     </row>
-    <row r="330" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A330" s="28"/>
       <c r="B330" s="38">
         <v>43644</v>
@@ -53361,7 +53356,7 @@
       </c>
       <c r="AS330" s="28"/>
     </row>
-    <row r="331" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A331" s="28"/>
       <c r="B331" s="38">
         <v>43644</v>
@@ -53494,7 +53489,7 @@
       </c>
       <c r="AS331" s="28"/>
     </row>
-    <row r="332" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A332" s="28"/>
       <c r="B332" s="38">
         <v>43644</v>
@@ -53627,7 +53622,7 @@
       </c>
       <c r="AS332" s="28"/>
     </row>
-    <row r="333" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A333" s="28"/>
       <c r="B333" s="38">
         <v>43767</v>
@@ -53758,7 +53753,7 @@
       </c>
       <c r="AS333" s="28"/>
     </row>
-    <row r="334" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A334" s="28"/>
       <c r="B334" s="38">
         <v>43848</v>
@@ -53891,7 +53886,7 @@
       </c>
       <c r="AS334" s="28"/>
     </row>
-    <row r="335" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A335" s="28"/>
       <c r="B335" s="38">
         <v>43848</v>
@@ -54024,7 +54019,7 @@
       </c>
       <c r="AS335" s="28"/>
     </row>
-    <row r="336" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A336" s="28"/>
       <c r="B336" s="38">
         <v>43928</v>
@@ -54157,7 +54152,7 @@
       </c>
       <c r="AS336" s="28"/>
     </row>
-    <row r="337" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A337" s="28"/>
       <c r="B337" s="38">
         <v>44054</v>
@@ -54290,7 +54285,7 @@
       </c>
       <c r="AS337" s="28"/>
     </row>
-    <row r="338" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A338" s="28"/>
       <c r="B338" s="38">
         <v>44054</v>
@@ -54423,7 +54418,7 @@
       </c>
       <c r="AS338" s="28"/>
     </row>
-    <row r="339" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A339" s="28"/>
       <c r="B339" s="38">
         <v>44054</v>
@@ -54556,7 +54551,7 @@
       </c>
       <c r="AS339" s="28"/>
     </row>
-    <row r="340" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A340" s="28"/>
       <c r="B340" s="38">
         <v>44173</v>
@@ -54689,7 +54684,7 @@
       </c>
       <c r="AS340" s="28"/>
     </row>
-    <row r="341" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A341" s="28"/>
       <c r="B341" s="38">
         <v>44173</v>
@@ -54822,7 +54817,7 @@
       </c>
       <c r="AS341" s="28"/>
     </row>
-    <row r="342" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A342" s="28"/>
       <c r="B342" s="38">
         <v>44173</v>
@@ -54955,7 +54950,7 @@
       </c>
       <c r="AS342" s="28"/>
     </row>
-    <row r="343" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A343" s="28"/>
       <c r="B343" s="29">
         <v>44299</v>
@@ -55086,7 +55081,7 @@
       </c>
       <c r="AS343" s="28"/>
     </row>
-    <row r="344" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A344" s="28"/>
       <c r="B344" s="29">
         <v>44299</v>
@@ -55217,7 +55212,7 @@
       </c>
       <c r="AS344" s="28"/>
     </row>
-    <row r="345" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A345" s="28"/>
       <c r="B345" s="29">
         <v>44299</v>
@@ -55346,7 +55341,7 @@
       </c>
       <c r="AS345" s="28"/>
     </row>
-    <row r="346" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A346" s="28" t="s">
         <v>780</v>
       </c>
@@ -59859,7 +59854,7 @@
         <v>782</v>
       </c>
       <c r="F382" s="28" t="s">
-        <v>3395</v>
+        <v>3394</v>
       </c>
       <c r="G382" s="28" t="s">
         <v>3081</v>
@@ -62202,7 +62197,7 @@
         <v>3332</v>
       </c>
       <c r="H403" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I403" s="87" t="s">
         <v>3333</v>
@@ -62270,7 +62265,7 @@
         <v>87</v>
       </c>
       <c r="AR403" s="87" t="s">
-        <v>3379</v>
+        <v>3378</v>
       </c>
       <c r="AS403" s="87"/>
     </row>
@@ -62323,7 +62318,7 @@
       <c r="AR404" s="87"/>
       <c r="AS404" s="87"/>
     </row>
-    <row r="405" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A405" s="87"/>
       <c r="B405" s="88">
         <v>44537</v>
@@ -62452,7 +62447,7 @@
       </c>
       <c r="AS405" s="87"/>
     </row>
-    <row r="406" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A406" s="87"/>
       <c r="B406" s="88">
         <v>44537</v>
@@ -62581,7 +62576,7 @@
       </c>
       <c r="AS406" s="87"/>
     </row>
-    <row r="407" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A407" s="87"/>
       <c r="B407" s="88">
         <v>44537</v>
@@ -62710,7 +62705,7 @@
       </c>
       <c r="AS407" s="87"/>
     </row>
-    <row r="408" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A408" s="87"/>
       <c r="B408" s="88">
         <v>44537</v>
@@ -62839,7 +62834,7 @@
       </c>
       <c r="AS408" s="87"/>
     </row>
-    <row r="409" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A409" s="87"/>
       <c r="B409" s="88">
         <v>44537</v>
@@ -62968,7 +62963,7 @@
       </c>
       <c r="AS409" s="87"/>
     </row>
-    <row r="410" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A410" s="87"/>
       <c r="B410" s="88">
         <v>44663</v>
@@ -62989,7 +62984,7 @@
         <v>3338</v>
       </c>
       <c r="H410" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I410" s="87" t="s">
         <v>3333</v>
@@ -63057,11 +63052,11 @@
         <v>20083</v>
       </c>
       <c r="AR410" s="87" t="s">
-        <v>3380</v>
+        <v>3379</v>
       </c>
       <c r="AS410" s="87"/>
     </row>
-    <row r="411" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A411" s="87"/>
       <c r="B411" s="88">
         <v>44663</v>
@@ -63082,7 +63077,7 @@
         <v>3342</v>
       </c>
       <c r="H411" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I411" s="87" t="s">
         <v>3333</v>
@@ -63150,11 +63145,11 @@
         <v>20082</v>
       </c>
       <c r="AR411" s="87" t="s">
-        <v>3381</v>
+        <v>3380</v>
       </c>
       <c r="AS411" s="87"/>
     </row>
-    <row r="412" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A412" s="87"/>
       <c r="B412" s="88">
         <v>44663</v>
@@ -63175,13 +63170,13 @@
         <v>3346</v>
       </c>
       <c r="H412" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I412" s="87" t="s">
         <v>3333</v>
       </c>
       <c r="J412" s="87" t="s">
-        <v>3347</v>
+        <v>1538</v>
       </c>
       <c r="K412" s="87" t="s">
         <v>3091</v>
@@ -63222,7 +63217,7 @@
         <v>186</v>
       </c>
       <c r="AK412" s="87" t="s">
-        <v>3348</v>
+        <v>3347</v>
       </c>
       <c r="AL412" s="87" t="s">
         <v>1146</v>
@@ -63243,11 +63238,11 @@
         <v>64004</v>
       </c>
       <c r="AR412" s="87" t="s">
-        <v>3382</v>
+        <v>3381</v>
       </c>
       <c r="AS412" s="87"/>
     </row>
-    <row r="413" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A413" s="87" t="s">
         <v>3200</v>
       </c>
@@ -63296,7 +63291,7 @@
       <c r="AR413" s="87"/>
       <c r="AS413" s="87"/>
     </row>
-    <row r="414" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A414" s="87"/>
       <c r="B414" s="88">
         <v>44663</v>
@@ -63305,19 +63300,19 @@
         <v>136</v>
       </c>
       <c r="D414" s="87" t="s">
-        <v>3375</v>
+        <v>3374</v>
       </c>
       <c r="E414" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F414" s="87" t="s">
+        <v>3375</v>
+      </c>
+      <c r="G414" s="87" t="s">
         <v>3376</v>
       </c>
-      <c r="G414" s="87" t="s">
-        <v>3377</v>
-      </c>
       <c r="H414" s="91" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I414" s="87" t="s">
         <v>3333</v>
@@ -63364,7 +63359,7 @@
         <v>574</v>
       </c>
       <c r="AK414" s="87" t="s">
-        <v>3378</v>
+        <v>3377</v>
       </c>
       <c r="AL414" s="87" t="s">
         <v>925</v>
@@ -63385,11 +63380,11 @@
         <v>30115</v>
       </c>
       <c r="AR414" s="87" t="s">
-        <v>3375</v>
+        <v>3374</v>
       </c>
       <c r="AS414" s="87"/>
     </row>
-    <row r="415" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A415" s="87"/>
       <c r="B415" s="88">
         <v>44551</v>
@@ -63522,7 +63517,7 @@
       </c>
       <c r="AS415" s="87"/>
     </row>
-    <row r="416" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A416" s="87"/>
       <c r="B416" s="88">
         <v>44551</v>
@@ -63655,7 +63650,7 @@
       </c>
       <c r="AS416" s="87"/>
     </row>
-    <row r="417" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A417" s="87"/>
       <c r="B417" s="88">
         <v>44551</v>
@@ -63788,7 +63783,7 @@
       </c>
       <c r="AS417" s="87"/>
     </row>
-    <row r="418" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A418" s="87"/>
       <c r="B418" s="88">
         <v>44551</v>
@@ -63921,7 +63916,7 @@
       </c>
       <c r="AS418" s="87"/>
     </row>
-    <row r="419" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A419" s="87"/>
       <c r="B419" s="88">
         <v>44565</v>
@@ -64054,7 +64049,7 @@
       </c>
       <c r="AS419" s="87"/>
     </row>
-    <row r="420" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A420" s="87"/>
       <c r="B420" s="88">
         <v>44565</v>
@@ -64187,7 +64182,7 @@
       </c>
       <c r="AS420" s="87"/>
     </row>
-    <row r="421" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A421" s="87"/>
       <c r="B421" s="88">
         <v>44565</v>
@@ -64320,7 +64315,7 @@
       </c>
       <c r="AS421" s="87"/>
     </row>
-    <row r="422" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A422" s="87"/>
       <c r="B422" s="88">
         <v>44565</v>
@@ -64453,7 +64448,7 @@
       </c>
       <c r="AS422" s="87"/>
     </row>
-    <row r="423" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A423" s="87"/>
       <c r="B423" s="88">
         <v>44677</v>
@@ -64462,19 +64457,19 @@
         <v>137</v>
       </c>
       <c r="D423" s="87" t="s">
-        <v>3389</v>
+        <v>3388</v>
       </c>
       <c r="E423" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F423" s="87" t="s">
+        <v>3389</v>
+      </c>
+      <c r="G423" s="87" t="s">
         <v>3390</v>
       </c>
-      <c r="G423" s="87" t="s">
-        <v>3391</v>
-      </c>
       <c r="H423" s="89" t="s">
-        <v>3393</v>
+        <v>3392</v>
       </c>
       <c r="I423" s="87" t="s">
         <v>3333</v>
@@ -64521,10 +64516,10 @@
         <v>3325</v>
       </c>
       <c r="AK423" s="87" t="s">
-        <v>3392</v>
+        <v>3391</v>
       </c>
       <c r="AL423" s="87" t="s">
-        <v>3397</v>
+        <v>3396</v>
       </c>
       <c r="AM423" s="87" t="s">
         <v>925</v>
@@ -64533,7 +64528,7 @@
         <v>925</v>
       </c>
       <c r="AO423" s="87" t="s">
-        <v>3394</v>
+        <v>3393</v>
       </c>
       <c r="AP423" s="87">
         <v>30106</v>
@@ -64542,11 +64537,11 @@
         <v>30106</v>
       </c>
       <c r="AR423" s="87" t="s">
-        <v>3396</v>
+        <v>3395</v>
       </c>
       <c r="AS423" s="87"/>
     </row>
-    <row r="424" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:45" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A424" s="87" t="s">
         <v>3199</v>
       </c>
@@ -64604,19 +64599,19 @@
         <v>0</v>
       </c>
       <c r="D425" s="87" t="s">
-        <v>3350</v>
+        <v>3349</v>
       </c>
       <c r="E425" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F425" s="87" t="s">
+        <v>3350</v>
+      </c>
+      <c r="G425" s="87" t="s">
         <v>3351</v>
       </c>
-      <c r="G425" s="87" t="s">
-        <v>3352</v>
-      </c>
       <c r="H425" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I425" s="87" t="s">
         <v>3333</v>
@@ -64625,7 +64620,7 @@
         <v>75</v>
       </c>
       <c r="K425" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L425" s="87">
         <v>0</v>
@@ -64663,7 +64658,7 @@
         <v>575</v>
       </c>
       <c r="AK425" s="87" t="s">
-        <v>3354</v>
+        <v>3353</v>
       </c>
       <c r="AL425" s="87" t="s">
         <v>925</v>
@@ -64691,19 +64686,19 @@
         <v>0</v>
       </c>
       <c r="D426" s="87" t="s">
-        <v>3355</v>
+        <v>3354</v>
       </c>
       <c r="E426" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F426" s="87" t="s">
+        <v>3355</v>
+      </c>
+      <c r="G426" s="87" t="s">
         <v>3356</v>
       </c>
-      <c r="G426" s="87" t="s">
-        <v>3357</v>
-      </c>
       <c r="H426" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I426" s="87" t="s">
         <v>3333</v>
@@ -64712,7 +64707,7 @@
         <v>75</v>
       </c>
       <c r="K426" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L426" s="87">
         <v>0</v>
@@ -64750,7 +64745,7 @@
         <v>575</v>
       </c>
       <c r="AK426" s="87" t="s">
-        <v>3358</v>
+        <v>3357</v>
       </c>
       <c r="AL426" s="87" t="s">
         <v>925</v>
@@ -64778,19 +64773,19 @@
         <v>0</v>
       </c>
       <c r="D427" s="87" t="s">
-        <v>3359</v>
+        <v>3358</v>
       </c>
       <c r="E427" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F427" s="87" t="s">
+        <v>3359</v>
+      </c>
+      <c r="G427" s="87" t="s">
         <v>3360</v>
       </c>
-      <c r="G427" s="87" t="s">
-        <v>3361</v>
-      </c>
       <c r="H427" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I427" s="87" t="s">
         <v>3333</v>
@@ -64799,7 +64794,7 @@
         <v>75</v>
       </c>
       <c r="K427" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L427" s="87">
         <v>0</v>
@@ -64837,7 +64832,7 @@
         <v>575</v>
       </c>
       <c r="AK427" s="87" t="s">
-        <v>3362</v>
+        <v>3361</v>
       </c>
       <c r="AL427" s="87" t="s">
         <v>925</v>
@@ -64865,19 +64860,19 @@
         <v>1</v>
       </c>
       <c r="D428" s="87" t="s">
-        <v>3363</v>
+        <v>3362</v>
       </c>
       <c r="E428" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F428" s="87" t="s">
-        <v>3383</v>
+        <v>3382</v>
       </c>
       <c r="G428" s="87" t="s">
-        <v>3365</v>
+        <v>3364</v>
       </c>
       <c r="H428" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I428" s="87" t="s">
         <v>3333</v>
@@ -64886,7 +64881,7 @@
         <v>75</v>
       </c>
       <c r="K428" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L428" s="87">
         <v>0</v>
@@ -64924,7 +64919,7 @@
         <v>575</v>
       </c>
       <c r="AK428" s="87" t="s">
-        <v>3366</v>
+        <v>3365</v>
       </c>
       <c r="AL428" s="87" t="s">
         <v>925</v>
@@ -64945,7 +64940,7 @@
     </row>
     <row r="429" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A429" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B429" s="88">
         <v>44663</v>
@@ -64954,19 +64949,19 @@
         <v>0</v>
       </c>
       <c r="D429" s="87" t="s">
-        <v>3363</v>
+        <v>3362</v>
       </c>
       <c r="E429" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F429" s="87" t="s">
+        <v>3363</v>
+      </c>
+      <c r="G429" s="87" t="s">
         <v>3364</v>
       </c>
-      <c r="G429" s="87" t="s">
-        <v>3365</v>
-      </c>
       <c r="H429" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I429" s="87" t="s">
         <v>3333</v>
@@ -64975,7 +64970,7 @@
         <v>75</v>
       </c>
       <c r="K429" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L429" s="87">
         <v>0</v>
@@ -65013,7 +65008,7 @@
         <v>575</v>
       </c>
       <c r="AK429" s="87" t="s">
-        <v>3366</v>
+        <v>3365</v>
       </c>
       <c r="AL429" s="87" t="s">
         <v>925</v>
@@ -65034,7 +65029,7 @@
     </row>
     <row r="430" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A430" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B430" s="88">
         <v>44663</v>
@@ -65043,19 +65038,19 @@
         <v>0</v>
       </c>
       <c r="D430" s="87" t="s">
-        <v>3363</v>
+        <v>3362</v>
       </c>
       <c r="E430" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F430" s="87" t="s">
+        <v>3363</v>
+      </c>
+      <c r="G430" s="87" t="s">
         <v>3364</v>
       </c>
-      <c r="G430" s="87" t="s">
-        <v>3365</v>
-      </c>
       <c r="H430" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I430" s="87" t="s">
         <v>3333</v>
@@ -65064,7 +65059,7 @@
         <v>75</v>
       </c>
       <c r="K430" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L430" s="87">
         <v>0</v>
@@ -65102,7 +65097,7 @@
         <v>575</v>
       </c>
       <c r="AK430" s="87" t="s">
-        <v>3366</v>
+        <v>3365</v>
       </c>
       <c r="AL430" s="87" t="s">
         <v>925</v>
@@ -65130,19 +65125,19 @@
         <v>2</v>
       </c>
       <c r="D431" s="87" t="s">
-        <v>3363</v>
+        <v>3362</v>
       </c>
       <c r="E431" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F431" s="87" t="s">
-        <v>3384</v>
+        <v>3383</v>
       </c>
       <c r="G431" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H431" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I431" s="87" t="s">
         <v>3333</v>
@@ -65151,7 +65146,7 @@
         <v>75</v>
       </c>
       <c r="K431" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L431" s="87">
         <v>0</v>
@@ -65189,7 +65184,7 @@
         <v>575</v>
       </c>
       <c r="AK431" s="87" t="s">
-        <v>3366</v>
+        <v>3365</v>
       </c>
       <c r="AL431" s="87" t="s">
         <v>925</v>
@@ -65210,7 +65205,7 @@
     </row>
     <row r="432" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A432" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B432" s="88">
         <v>44663</v>
@@ -65219,19 +65214,19 @@
         <v>0</v>
       </c>
       <c r="D432" s="87" t="s">
-        <v>3363</v>
+        <v>3362</v>
       </c>
       <c r="E432" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F432" s="87" t="s">
-        <v>3364</v>
+        <v>3363</v>
       </c>
       <c r="G432" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H432" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I432" s="87" t="s">
         <v>3333</v>
@@ -65240,7 +65235,7 @@
         <v>75</v>
       </c>
       <c r="K432" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L432" s="87">
         <v>0</v>
@@ -65278,7 +65273,7 @@
         <v>575</v>
       </c>
       <c r="AK432" s="87" t="s">
-        <v>3366</v>
+        <v>3365</v>
       </c>
       <c r="AL432" s="87" t="s">
         <v>925</v>
@@ -65299,7 +65294,7 @@
     </row>
     <row r="433" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A433" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B433" s="88">
         <v>44663</v>
@@ -65308,19 +65303,19 @@
         <v>0</v>
       </c>
       <c r="D433" s="87" t="s">
-        <v>3363</v>
+        <v>3362</v>
       </c>
       <c r="E433" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F433" s="87" t="s">
-        <v>3364</v>
+        <v>3363</v>
       </c>
       <c r="G433" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H433" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I433" s="87" t="s">
         <v>3333</v>
@@ -65329,7 +65324,7 @@
         <v>75</v>
       </c>
       <c r="K433" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L433" s="87">
         <v>0</v>
@@ -65367,7 +65362,7 @@
         <v>575</v>
       </c>
       <c r="AK433" s="87" t="s">
-        <v>3366</v>
+        <v>3365</v>
       </c>
       <c r="AL433" s="87" t="s">
         <v>925</v>
@@ -65388,7 +65383,7 @@
     </row>
     <row r="434" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A434" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B434" s="88">
         <v>44663</v>
@@ -65397,19 +65392,19 @@
         <v>0</v>
       </c>
       <c r="D434" s="87" t="s">
-        <v>3363</v>
+        <v>3362</v>
       </c>
       <c r="E434" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F434" s="87" t="s">
-        <v>3364</v>
+        <v>3363</v>
       </c>
       <c r="G434" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H434" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I434" s="87" t="s">
         <v>3333</v>
@@ -65418,7 +65413,7 @@
         <v>75</v>
       </c>
       <c r="K434" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L434" s="87">
         <v>0</v>
@@ -65456,7 +65451,7 @@
         <v>575</v>
       </c>
       <c r="AK434" s="87" t="s">
-        <v>3366</v>
+        <v>3365</v>
       </c>
       <c r="AL434" s="87" t="s">
         <v>925</v>
@@ -65477,7 +65472,7 @@
     </row>
     <row r="435" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A435" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B435" s="88">
         <v>44663</v>
@@ -65486,19 +65481,19 @@
         <v>0</v>
       </c>
       <c r="D435" s="87" t="s">
-        <v>3363</v>
+        <v>3362</v>
       </c>
       <c r="E435" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F435" s="87" t="s">
-        <v>3364</v>
+        <v>3363</v>
       </c>
       <c r="G435" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H435" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I435" s="87" t="s">
         <v>3333</v>
@@ -65507,7 +65502,7 @@
         <v>75</v>
       </c>
       <c r="K435" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L435" s="87">
         <v>0</v>
@@ -65545,7 +65540,7 @@
         <v>575</v>
       </c>
       <c r="AK435" s="87" t="s">
-        <v>3366</v>
+        <v>3365</v>
       </c>
       <c r="AL435" s="87" t="s">
         <v>925</v>
@@ -65573,19 +65568,19 @@
         <v>3</v>
       </c>
       <c r="D436" s="87" t="s">
-        <v>3368</v>
+        <v>3367</v>
       </c>
       <c r="E436" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F436" s="87" t="s">
-        <v>3385</v>
+        <v>3384</v>
       </c>
       <c r="G436" s="87" t="s">
-        <v>3365</v>
+        <v>3364</v>
       </c>
       <c r="H436" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I436" s="87" t="s">
         <v>3333</v>
@@ -65594,7 +65589,7 @@
         <v>75</v>
       </c>
       <c r="K436" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L436" s="87">
         <v>0</v>
@@ -65632,7 +65627,7 @@
         <v>575</v>
       </c>
       <c r="AK436" s="87" t="s">
-        <v>3370</v>
+        <v>3369</v>
       </c>
       <c r="AL436" s="87" t="s">
         <v>925</v>
@@ -65653,7 +65648,7 @@
     </row>
     <row r="437" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A437" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B437" s="88">
         <v>44663</v>
@@ -65662,19 +65657,19 @@
         <v>0</v>
       </c>
       <c r="D437" s="87" t="s">
-        <v>3368</v>
+        <v>3367</v>
       </c>
       <c r="E437" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F437" s="87" t="s">
-        <v>3369</v>
+        <v>3368</v>
       </c>
       <c r="G437" s="87" t="s">
-        <v>3365</v>
+        <v>3364</v>
       </c>
       <c r="H437" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I437" s="87" t="s">
         <v>3333</v>
@@ -65683,7 +65678,7 @@
         <v>75</v>
       </c>
       <c r="K437" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L437" s="87">
         <v>0</v>
@@ -65721,7 +65716,7 @@
         <v>575</v>
       </c>
       <c r="AK437" s="87" t="s">
-        <v>3370</v>
+        <v>3369</v>
       </c>
       <c r="AL437" s="87" t="s">
         <v>925</v>
@@ -65742,7 +65737,7 @@
     </row>
     <row r="438" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A438" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B438" s="88">
         <v>44663</v>
@@ -65751,19 +65746,19 @@
         <v>0</v>
       </c>
       <c r="D438" s="87" t="s">
-        <v>3368</v>
+        <v>3367</v>
       </c>
       <c r="E438" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F438" s="87" t="s">
-        <v>3369</v>
+        <v>3368</v>
       </c>
       <c r="G438" s="87" t="s">
-        <v>3365</v>
+        <v>3364</v>
       </c>
       <c r="H438" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I438" s="87" t="s">
         <v>3333</v>
@@ -65772,7 +65767,7 @@
         <v>75</v>
       </c>
       <c r="K438" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L438" s="87">
         <v>0</v>
@@ -65810,7 +65805,7 @@
         <v>575</v>
       </c>
       <c r="AK438" s="87" t="s">
-        <v>3370</v>
+        <v>3369</v>
       </c>
       <c r="AL438" s="87" t="s">
         <v>925</v>
@@ -65838,19 +65833,19 @@
         <v>4</v>
       </c>
       <c r="D439" s="87" t="s">
-        <v>3368</v>
+        <v>3367</v>
       </c>
       <c r="E439" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F439" s="87" t="s">
-        <v>3386</v>
+        <v>3385</v>
       </c>
       <c r="G439" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H439" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I439" s="87" t="s">
         <v>3333</v>
@@ -65859,7 +65854,7 @@
         <v>75</v>
       </c>
       <c r="K439" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L439" s="87">
         <v>0</v>
@@ -65897,7 +65892,7 @@
         <v>575</v>
       </c>
       <c r="AK439" s="87" t="s">
-        <v>3370</v>
+        <v>3369</v>
       </c>
       <c r="AL439" s="87" t="s">
         <v>925</v>
@@ -65918,7 +65913,7 @@
     </row>
     <row r="440" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A440" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B440" s="88">
         <v>44663</v>
@@ -65927,19 +65922,19 @@
         <v>0</v>
       </c>
       <c r="D440" s="87" t="s">
-        <v>3368</v>
+        <v>3367</v>
       </c>
       <c r="E440" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F440" s="87" t="s">
-        <v>3369</v>
+        <v>3368</v>
       </c>
       <c r="G440" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H440" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I440" s="87" t="s">
         <v>3333</v>
@@ -65948,7 +65943,7 @@
         <v>75</v>
       </c>
       <c r="K440" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L440" s="87">
         <v>0</v>
@@ -65986,7 +65981,7 @@
         <v>575</v>
       </c>
       <c r="AK440" s="87" t="s">
-        <v>3370</v>
+        <v>3369</v>
       </c>
       <c r="AL440" s="87" t="s">
         <v>925</v>
@@ -66007,7 +66002,7 @@
     </row>
     <row r="441" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A441" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B441" s="88">
         <v>44663</v>
@@ -66016,19 +66011,19 @@
         <v>0</v>
       </c>
       <c r="D441" s="87" t="s">
-        <v>3368</v>
+        <v>3367</v>
       </c>
       <c r="E441" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F441" s="87" t="s">
-        <v>3369</v>
+        <v>3368</v>
       </c>
       <c r="G441" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H441" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I441" s="87" t="s">
         <v>3333</v>
@@ -66037,7 +66032,7 @@
         <v>75</v>
       </c>
       <c r="K441" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L441" s="87">
         <v>0</v>
@@ -66075,7 +66070,7 @@
         <v>575</v>
       </c>
       <c r="AK441" s="87" t="s">
-        <v>3370</v>
+        <v>3369</v>
       </c>
       <c r="AL441" s="87" t="s">
         <v>925</v>
@@ -66096,7 +66091,7 @@
     </row>
     <row r="442" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A442" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B442" s="88">
         <v>44663</v>
@@ -66105,19 +66100,19 @@
         <v>0</v>
       </c>
       <c r="D442" s="87" t="s">
-        <v>3368</v>
+        <v>3367</v>
       </c>
       <c r="E442" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F442" s="87" t="s">
-        <v>3369</v>
+        <v>3368</v>
       </c>
       <c r="G442" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H442" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I442" s="87" t="s">
         <v>3333</v>
@@ -66126,7 +66121,7 @@
         <v>75</v>
       </c>
       <c r="K442" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L442" s="87">
         <v>0</v>
@@ -66164,7 +66159,7 @@
         <v>575</v>
       </c>
       <c r="AK442" s="87" t="s">
-        <v>3370</v>
+        <v>3369</v>
       </c>
       <c r="AL442" s="87" t="s">
         <v>925</v>
@@ -66185,7 +66180,7 @@
     </row>
     <row r="443" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A443" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B443" s="88">
         <v>44663</v>
@@ -66194,19 +66189,19 @@
         <v>0</v>
       </c>
       <c r="D443" s="87" t="s">
-        <v>3368</v>
+        <v>3367</v>
       </c>
       <c r="E443" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F443" s="87" t="s">
-        <v>3369</v>
+        <v>3368</v>
       </c>
       <c r="G443" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H443" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I443" s="87" t="s">
         <v>3333</v>
@@ -66215,7 +66210,7 @@
         <v>75</v>
       </c>
       <c r="K443" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L443" s="87">
         <v>0</v>
@@ -66253,7 +66248,7 @@
         <v>575</v>
       </c>
       <c r="AK443" s="87" t="s">
-        <v>3370</v>
+        <v>3369</v>
       </c>
       <c r="AL443" s="87" t="s">
         <v>925</v>
@@ -66281,19 +66276,19 @@
         <v>5</v>
       </c>
       <c r="D444" s="87" t="s">
-        <v>3371</v>
+        <v>3370</v>
       </c>
       <c r="E444" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F444" s="87" t="s">
-        <v>3387</v>
+        <v>3386</v>
       </c>
       <c r="G444" s="87" t="s">
-        <v>3365</v>
+        <v>3364</v>
       </c>
       <c r="H444" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I444" s="87" t="s">
         <v>3333</v>
@@ -66302,7 +66297,7 @@
         <v>75</v>
       </c>
       <c r="K444" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L444" s="87">
         <v>0</v>
@@ -66340,7 +66335,7 @@
         <v>575</v>
       </c>
       <c r="AK444" s="87" t="s">
-        <v>3373</v>
+        <v>3372</v>
       </c>
       <c r="AL444" s="87" t="s">
         <v>925</v>
@@ -66361,7 +66356,7 @@
     </row>
     <row r="445" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A445" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B445" s="88">
         <v>44663</v>
@@ -66370,19 +66365,19 @@
         <v>0</v>
       </c>
       <c r="D445" s="87" t="s">
-        <v>3371</v>
+        <v>3370</v>
       </c>
       <c r="E445" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F445" s="87" t="s">
-        <v>3372</v>
+        <v>3371</v>
       </c>
       <c r="G445" s="87" t="s">
-        <v>3365</v>
+        <v>3364</v>
       </c>
       <c r="H445" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I445" s="87" t="s">
         <v>3333</v>
@@ -66391,7 +66386,7 @@
         <v>75</v>
       </c>
       <c r="K445" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L445" s="87">
         <v>0</v>
@@ -66429,7 +66424,7 @@
         <v>575</v>
       </c>
       <c r="AK445" s="87" t="s">
-        <v>3373</v>
+        <v>3372</v>
       </c>
       <c r="AL445" s="87" t="s">
         <v>925</v>
@@ -66450,7 +66445,7 @@
     </row>
     <row r="446" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A446" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B446" s="88">
         <v>44663</v>
@@ -66459,19 +66454,19 @@
         <v>0</v>
       </c>
       <c r="D446" s="87" t="s">
-        <v>3371</v>
+        <v>3370</v>
       </c>
       <c r="E446" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F446" s="87" t="s">
-        <v>3372</v>
+        <v>3371</v>
       </c>
       <c r="G446" s="87" t="s">
-        <v>3365</v>
+        <v>3364</v>
       </c>
       <c r="H446" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I446" s="87" t="s">
         <v>3333</v>
@@ -66480,7 +66475,7 @@
         <v>75</v>
       </c>
       <c r="K446" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L446" s="87">
         <v>0</v>
@@ -66518,7 +66513,7 @@
         <v>575</v>
       </c>
       <c r="AK446" s="87" t="s">
-        <v>3373</v>
+        <v>3372</v>
       </c>
       <c r="AL446" s="87" t="s">
         <v>925</v>
@@ -66546,19 +66541,19 @@
         <v>6</v>
       </c>
       <c r="D447" s="87" t="s">
-        <v>3371</v>
+        <v>3370</v>
       </c>
       <c r="E447" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F447" s="87" t="s">
-        <v>3388</v>
+        <v>3387</v>
       </c>
       <c r="G447" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H447" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I447" s="87" t="s">
         <v>3333</v>
@@ -66567,7 +66562,7 @@
         <v>75</v>
       </c>
       <c r="K447" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L447" s="87">
         <v>0</v>
@@ -66605,7 +66600,7 @@
         <v>575</v>
       </c>
       <c r="AK447" s="87" t="s">
-        <v>3373</v>
+        <v>3372</v>
       </c>
       <c r="AL447" s="87" t="s">
         <v>925</v>
@@ -66626,7 +66621,7 @@
     </row>
     <row r="448" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A448" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B448" s="88">
         <v>44663</v>
@@ -66635,19 +66630,19 @@
         <v>0</v>
       </c>
       <c r="D448" s="87" t="s">
-        <v>3371</v>
+        <v>3370</v>
       </c>
       <c r="E448" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F448" s="87" t="s">
-        <v>3372</v>
+        <v>3371</v>
       </c>
       <c r="G448" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H448" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I448" s="87" t="s">
         <v>3333</v>
@@ -66656,7 +66651,7 @@
         <v>75</v>
       </c>
       <c r="K448" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L448" s="87">
         <v>0</v>
@@ -66694,7 +66689,7 @@
         <v>575</v>
       </c>
       <c r="AK448" s="87" t="s">
-        <v>3373</v>
+        <v>3372</v>
       </c>
       <c r="AL448" s="87" t="s">
         <v>925</v>
@@ -66715,7 +66710,7 @@
     </row>
     <row r="449" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A449" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B449" s="88">
         <v>44663</v>
@@ -66724,19 +66719,19 @@
         <v>0</v>
       </c>
       <c r="D449" s="87" t="s">
-        <v>3371</v>
+        <v>3370</v>
       </c>
       <c r="E449" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F449" s="87" t="s">
-        <v>3372</v>
+        <v>3371</v>
       </c>
       <c r="G449" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H449" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I449" s="87" t="s">
         <v>3333</v>
@@ -66745,7 +66740,7 @@
         <v>75</v>
       </c>
       <c r="K449" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L449" s="87">
         <v>0</v>
@@ -66783,7 +66778,7 @@
         <v>575</v>
       </c>
       <c r="AK449" s="87" t="s">
-        <v>3373</v>
+        <v>3372</v>
       </c>
       <c r="AL449" s="87" t="s">
         <v>925</v>
@@ -66804,7 +66799,7 @@
     </row>
     <row r="450" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A450" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B450" s="88">
         <v>44663</v>
@@ -66813,19 +66808,19 @@
         <v>0</v>
       </c>
       <c r="D450" s="87" t="s">
-        <v>3371</v>
+        <v>3370</v>
       </c>
       <c r="E450" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F450" s="87" t="s">
-        <v>3372</v>
+        <v>3371</v>
       </c>
       <c r="G450" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H450" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I450" s="87" t="s">
         <v>3333</v>
@@ -66834,7 +66829,7 @@
         <v>75</v>
       </c>
       <c r="K450" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L450" s="87">
         <v>0</v>
@@ -66872,7 +66867,7 @@
         <v>575</v>
       </c>
       <c r="AK450" s="87" t="s">
-        <v>3373</v>
+        <v>3372</v>
       </c>
       <c r="AL450" s="87" t="s">
         <v>925</v>
@@ -66893,7 +66888,7 @@
     </row>
     <row r="451" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A451" s="87" t="s">
-        <v>3374</v>
+        <v>3373</v>
       </c>
       <c r="B451" s="88">
         <v>44663</v>
@@ -66902,19 +66897,19 @@
         <v>0</v>
       </c>
       <c r="D451" s="87" t="s">
-        <v>3371</v>
+        <v>3370</v>
       </c>
       <c r="E451" s="87" t="s">
         <v>3085</v>
       </c>
       <c r="F451" s="87" t="s">
-        <v>3372</v>
+        <v>3371</v>
       </c>
       <c r="G451" s="87" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="H451" s="89" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I451" s="87" t="s">
         <v>3333</v>
@@ -66923,7 +66918,7 @@
         <v>75</v>
       </c>
       <c r="K451" s="87" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="L451" s="87">
         <v>0</v>
@@ -66961,7 +66956,7 @@
         <v>575</v>
       </c>
       <c r="AK451" s="87" t="s">
-        <v>3373</v>
+        <v>3372</v>
       </c>
       <c r="AL451" s="87" t="s">
         <v>925</v>

</xml_diff>